<commit_message>
:pencil: Updated sesio 4 new do files
</commit_message>
<xml_diff>
--- a/outputs/03-construccion-datos/duplicates/duplicates.xlsx
+++ b/outputs/03-construccion-datos/duplicates/duplicates.xlsx
@@ -24,7 +24,7 @@
     <t>datelisted</t>
   </si>
   <si>
-    <t>11Jul2020</t>
+    <t>12Jul2020</t>
   </si>
   <si>
     <t>datefixed</t>
@@ -497,154 +497,154 @@
         <v>1978</v>
       </c>
       <c r="K2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" s="1">
         <v>0</v>
       </c>
       <c r="O2" s="2">
-        <v>6.6651544570922852</v>
+        <v>8.5906248092651367</v>
       </c>
       <c r="P2" s="2">
-        <v>30.334941864013672</v>
+        <v>14.050758361816406</v>
       </c>
       <c r="Q2" s="2">
-        <v>37.171989440917969</v>
+        <v>12.506132125854492</v>
       </c>
       <c r="R2" s="2">
-        <v>8.207484245300293</v>
+        <v>14.704978942871094</v>
       </c>
       <c r="S2" s="2">
-        <v>34.572284698486328</v>
+        <v>15.732240676879883</v>
       </c>
       <c r="T2" s="2">
-        <v>2.8522243499755859</v>
+        <v>35.372631072998047</v>
       </c>
       <c r="U2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2" s="1">
         <v>1</v>
       </c>
       <c r="W2" s="2">
-        <v>2.0191493034362793</v>
+        <v>3.9138941764831543</v>
       </c>
       <c r="X2" s="2">
-        <v>36.617568969726563</v>
+        <v>13.375571250915527</v>
       </c>
       <c r="Y2" s="2">
-        <v>26.243560791015625</v>
+        <v>44.65960693359375</v>
       </c>
       <c r="Z2" s="2">
-        <v>2.6016087532043457</v>
+        <v>7.6776456832885742</v>
       </c>
       <c r="AA2" s="2">
-        <v>46.726428985595703</v>
+        <v>38.660953521728516</v>
       </c>
       <c r="AB2" s="2">
-        <v>42.202613830566406</v>
+        <v>30.264581680297852</v>
       </c>
       <c r="AC2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD2" s="1">
         <v>1</v>
       </c>
       <c r="AE2" s="2">
-        <v>14.696352005004883</v>
+        <v>19.735282897949219</v>
       </c>
       <c r="AF2" s="2">
-        <v>28.696521759033203</v>
+        <v>39.1041259765625</v>
       </c>
       <c r="AG2" s="2">
-        <v>10.950985908508301</v>
+        <v>3.3548846244812012</v>
       </c>
       <c r="AH2" s="2">
-        <v>13.345341682434082</v>
+        <v>4.9948983192443848</v>
       </c>
       <c r="AI2" s="2">
-        <v>20.124269485473633</v>
+        <v>31.555620193481445</v>
       </c>
       <c r="AJ2" s="2">
-        <v>34.889377593994141</v>
+        <v>8.9748449325561523</v>
       </c>
       <c r="AK2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL2" s="1">
         <v>1</v>
       </c>
       <c r="AM2" s="2">
-        <v>15.591218948364258</v>
+        <v>3.3343899250030518</v>
       </c>
       <c r="AN2" s="2">
-        <v>23.990056991577148</v>
+        <v>12.788989067077637</v>
       </c>
       <c r="AO2" s="2">
-        <v>19.519472122192383</v>
+        <v>32.278564453125</v>
       </c>
       <c r="AP2" s="2">
-        <v>4.1971988677978516</v>
+        <v>12.842391967773438</v>
       </c>
       <c r="AQ2" s="2">
-        <v>31.856826782226563</v>
+        <v>7.2027759552001953</v>
       </c>
       <c r="AR2" s="2">
-        <v>35.760978698730469</v>
+        <v>37.126541137695313</v>
       </c>
       <c r="AS2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU2" s="2">
-        <v>8.4271459579467773</v>
+        <v>14.665376663208008</v>
       </c>
       <c r="AV2" s="2">
-        <v>5.8868198394775391</v>
+        <v>4.4169931411743164</v>
       </c>
       <c r="AW2" s="2">
-        <v>8.0283241271972656</v>
+        <v>3.0003960132598877</v>
       </c>
       <c r="AX2" s="2">
-        <v>5.6476397514343262</v>
+        <v>8.2621965408325195</v>
       </c>
       <c r="AY2" s="2">
-        <v>19.629386901855469</v>
+        <v>49.364387512207031</v>
       </c>
       <c r="AZ2" s="2">
-        <v>47.574886322021484</v>
+        <v>46.937423706054688</v>
       </c>
       <c r="BA2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB2" s="1">
         <v>1</v>
       </c>
       <c r="BC2" s="2">
-        <v>13.528090476989746</v>
+        <v>1.1367254257202148</v>
       </c>
       <c r="BD2" s="2">
-        <v>36.350040435791016</v>
+        <v>20.284408569335938</v>
       </c>
       <c r="BE2" s="2">
-        <v>2.0229640007019043</v>
+        <v>30.025539398193359</v>
       </c>
       <c r="BF2" s="2">
-        <v>7.2983484268188477</v>
+        <v>5.3607869148254395</v>
       </c>
       <c r="BG2" s="2">
-        <v>12.92873477935791</v>
+        <v>34.062877655029297</v>
       </c>
       <c r="BH2" s="2">
-        <v>20.819072723388672</v>
+        <v>37.349773406982422</v>
       </c>
       <c r="BI2" t="s">
         <v>72</v>
@@ -680,154 +680,154 @@
         <v>2036</v>
       </c>
       <c r="K3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="1">
         <v>0</v>
       </c>
       <c r="O3" s="2">
-        <v>6.6651544570922852</v>
+        <v>8.5906248092651367</v>
       </c>
       <c r="P3" s="2">
-        <v>30.334941864013672</v>
+        <v>14.050758361816406</v>
       </c>
       <c r="Q3" s="2">
-        <v>37.171989440917969</v>
+        <v>12.506132125854492</v>
       </c>
       <c r="R3" s="2">
-        <v>8.207484245300293</v>
+        <v>14.704978942871094</v>
       </c>
       <c r="S3" s="2">
-        <v>34.572284698486328</v>
+        <v>15.732240676879883</v>
       </c>
       <c r="T3" s="2">
-        <v>2.8522243499755859</v>
+        <v>35.372631072998047</v>
       </c>
       <c r="U3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" s="1">
         <v>1</v>
       </c>
       <c r="W3" s="2">
-        <v>2.0191493034362793</v>
+        <v>3.9138941764831543</v>
       </c>
       <c r="X3" s="2">
-        <v>36.617568969726563</v>
+        <v>13.375571250915527</v>
       </c>
       <c r="Y3" s="2">
-        <v>26.243560791015625</v>
+        <v>44.65960693359375</v>
       </c>
       <c r="Z3" s="2">
-        <v>2.6016087532043457</v>
+        <v>7.6776456832885742</v>
       </c>
       <c r="AA3" s="2">
-        <v>46.726428985595703</v>
+        <v>38.660953521728516</v>
       </c>
       <c r="AB3" s="2">
-        <v>42.202613830566406</v>
+        <v>30.264581680297852</v>
       </c>
       <c r="AC3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3" s="1">
         <v>1</v>
       </c>
       <c r="AE3" s="2">
-        <v>14.696352005004883</v>
+        <v>19.735282897949219</v>
       </c>
       <c r="AF3" s="2">
-        <v>28.696521759033203</v>
+        <v>39.1041259765625</v>
       </c>
       <c r="AG3" s="2">
-        <v>10.950985908508301</v>
+        <v>3.3548846244812012</v>
       </c>
       <c r="AH3" s="2">
-        <v>13.345341682434082</v>
+        <v>4.9948983192443848</v>
       </c>
       <c r="AI3" s="2">
-        <v>20.124269485473633</v>
+        <v>31.555620193481445</v>
       </c>
       <c r="AJ3" s="2">
-        <v>34.889377593994141</v>
+        <v>8.9748449325561523</v>
       </c>
       <c r="AK3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL3" s="1">
         <v>1</v>
       </c>
       <c r="AM3" s="2">
-        <v>15.591218948364258</v>
+        <v>3.3343899250030518</v>
       </c>
       <c r="AN3" s="2">
-        <v>23.990056991577148</v>
+        <v>12.788989067077637</v>
       </c>
       <c r="AO3" s="2">
-        <v>19.519472122192383</v>
+        <v>32.278564453125</v>
       </c>
       <c r="AP3" s="2">
-        <v>4.1971988677978516</v>
+        <v>12.842391967773438</v>
       </c>
       <c r="AQ3" s="2">
-        <v>31.856826782226563</v>
+        <v>7.2027759552001953</v>
       </c>
       <c r="AR3" s="2">
-        <v>35.760978698730469</v>
+        <v>37.126541137695313</v>
       </c>
       <c r="AS3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU3" s="2">
-        <v>8.4271459579467773</v>
+        <v>14.665376663208008</v>
       </c>
       <c r="AV3" s="2">
-        <v>5.8868198394775391</v>
+        <v>4.4169931411743164</v>
       </c>
       <c r="AW3" s="2">
-        <v>8.0283241271972656</v>
+        <v>3.0003960132598877</v>
       </c>
       <c r="AX3" s="2">
-        <v>5.6476397514343262</v>
+        <v>8.2621965408325195</v>
       </c>
       <c r="AY3" s="2">
-        <v>19.629386901855469</v>
+        <v>49.364387512207031</v>
       </c>
       <c r="AZ3" s="2">
-        <v>47.574886322021484</v>
+        <v>46.937423706054688</v>
       </c>
       <c r="BA3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB3" s="1">
         <v>1</v>
       </c>
       <c r="BC3" s="2">
-        <v>13.528090476989746</v>
+        <v>1.1367254257202148</v>
       </c>
       <c r="BD3" s="2">
-        <v>36.350040435791016</v>
+        <v>20.284408569335938</v>
       </c>
       <c r="BE3" s="2">
-        <v>2.0229640007019043</v>
+        <v>30.025539398193359</v>
       </c>
       <c r="BF3" s="2">
-        <v>7.2983484268188477</v>
+        <v>5.3607869148254395</v>
       </c>
       <c r="BG3" s="2">
-        <v>12.92873477935791</v>
+        <v>34.062877655029297</v>
       </c>
       <c r="BH3" s="2">
-        <v>20.819072723388672</v>
+        <v>37.349773406982422</v>
       </c>
       <c r="BI3" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
:pencil: Updated papers and sesion 5 do files
</commit_message>
<xml_diff>
--- a/outputs/03-construccion-datos/duplicates/duplicates.xlsx
+++ b/outputs/03-construccion-datos/duplicates/duplicates.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>hhid</t>
   </si>
@@ -99,6 +99,9 @@
     <t>consum_kg_P1S1C1</t>
   </si>
   <si>
+    <t>sell_kg_P1S1C1</t>
+  </si>
+  <si>
     <t>seed_kg_P1S1C2</t>
   </si>
   <si>
@@ -108,6 +111,9 @@
     <t>consum_kg_P1S1C2</t>
   </si>
   <si>
+    <t>sell_kg_P1S1C2</t>
+  </si>
+  <si>
     <t>cult_P1S2</t>
   </si>
   <si>
@@ -123,6 +129,9 @@
     <t>consum_kg_P1S2C1</t>
   </si>
   <si>
+    <t>sell_kg_P1S2C1</t>
+  </si>
+  <si>
     <t>seed_kg_P1S2C2</t>
   </si>
   <si>
@@ -132,6 +141,9 @@
     <t>consum_kg_P1S2C2</t>
   </si>
   <si>
+    <t>sell_kg_P1S2C2</t>
+  </si>
+  <si>
     <t>cult_P1S3</t>
   </si>
   <si>
@@ -147,6 +159,9 @@
     <t>consum_kg_P1S3C1</t>
   </si>
   <si>
+    <t>sell_kg_P1S3C1</t>
+  </si>
+  <si>
     <t>seed_kg_P1S3C2</t>
   </si>
   <si>
@@ -156,6 +171,9 @@
     <t>consum_kg_P1S3C2</t>
   </si>
   <si>
+    <t>sell_kg_P1S3C2</t>
+  </si>
+  <si>
     <t>cult_P2S1</t>
   </si>
   <si>
@@ -171,6 +189,9 @@
     <t>consum_kg_P2S1C1</t>
   </si>
   <si>
+    <t>sell_kg_P2S1C1</t>
+  </si>
+  <si>
     <t>seed_kg_P2S1C2</t>
   </si>
   <si>
@@ -180,6 +201,9 @@
     <t>consum_kg_P2S1C2</t>
   </si>
   <si>
+    <t>sell_kg_P2S1C2</t>
+  </si>
+  <si>
     <t>cult_P2S2</t>
   </si>
   <si>
@@ -195,6 +219,9 @@
     <t>consum_kg_P2S2C1</t>
   </si>
   <si>
+    <t>sell_kg_P2S2C1</t>
+  </si>
+  <si>
     <t>seed_kg_P2S2C2</t>
   </si>
   <si>
@@ -204,6 +231,9 @@
     <t>consum_kg_P2S2C2</t>
   </si>
   <si>
+    <t>sell_kg_P2S2C2</t>
+  </si>
+  <si>
     <t>cult_P2S3</t>
   </si>
   <si>
@@ -219,6 +249,9 @@
     <t>consum_kg_P2S3C1</t>
   </si>
   <si>
+    <t>sell_kg_P2S3C1</t>
+  </si>
+  <si>
     <t>seed_kg_P2S3C2</t>
   </si>
   <si>
@@ -226,6 +259,15 @@
   </si>
   <si>
     <t>consum_kg_P2S3C2</t>
+  </si>
+  <si>
+    <t>sell_kg_P2S3C2</t>
+  </si>
+  <si>
+    <t>price_1</t>
+  </si>
+  <si>
+    <t>price_2</t>
   </si>
   <si>
     <t>listofdiffs</t>
@@ -279,7 +321,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BI3"/>
+  <dimension ref="A1:BW3"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -466,6 +508,48 @@
       <c r="BI1" t="s">
         <v>71</v>
       </c>
+      <c r="BJ1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -497,130 +581,130 @@
         <v>1978</v>
       </c>
       <c r="K2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L2" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
       </c>
       <c r="N2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" s="2">
-        <v>8.5906248092651367</v>
+        <v>3.1737830638885498</v>
       </c>
       <c r="P2" s="2">
-        <v>14.050758361816406</v>
+        <v>37.302322387695313</v>
       </c>
       <c r="Q2" s="2">
-        <v>12.506132125854492</v>
+        <v>27.001590728759766</v>
       </c>
       <c r="R2" s="2">
-        <v>14.704978942871094</v>
+        <v>10.300731658935547</v>
       </c>
       <c r="S2" s="2">
-        <v>15.732240676879883</v>
+        <v>9.8073272705078125</v>
       </c>
       <c r="T2" s="2">
-        <v>35.372631072998047</v>
-      </c>
-      <c r="U2" s="1">
-        <v>0</v>
-      </c>
-      <c r="V2" s="1">
+        <v>39.558097839355469</v>
+      </c>
+      <c r="U2" s="2">
+        <v>29.271829605102539</v>
+      </c>
+      <c r="V2" s="2">
+        <v>10.28626823425293</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1">
         <v>1</v>
       </c>
-      <c r="W2" s="2">
-        <v>3.9138941764831543</v>
-      </c>
-      <c r="X2" s="2">
-        <v>13.375571250915527</v>
-      </c>
       <c r="Y2" s="2">
-        <v>44.65960693359375</v>
+        <v>16.786825180053711</v>
       </c>
       <c r="Z2" s="2">
-        <v>7.6776456832885742</v>
+        <v>22.355806350708008</v>
       </c>
       <c r="AA2" s="2">
-        <v>38.660953521728516</v>
+        <v>22.355806350708008</v>
       </c>
       <c r="AB2" s="2">
-        <v>30.264581680297852</v>
-      </c>
-      <c r="AC2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>16.214475631713867</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>2.23555588722229</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>2.23555588722229</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>9.3099184036254883</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>45.388145446777344</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>34.738975524902344</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>10.649169921875</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>8.2044134140014648</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>33.867767333984375</v>
+      </c>
+      <c r="AO2" s="2">
+        <v>13.838119506835938</v>
+      </c>
+      <c r="AP2" s="2">
+        <v>20.029647827148438</v>
+      </c>
+      <c r="AQ2" s="1">
         <v>1</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AR2" s="1">
         <v>1</v>
       </c>
-      <c r="AE2" s="2">
-        <v>19.735282897949219</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>39.1041259765625</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>3.3548846244812012</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>4.9948983192443848</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>31.555620193481445</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>8.9748449325561523</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="2">
-        <v>3.3343899250030518</v>
-      </c>
-      <c r="AN2" s="2">
-        <v>12.788989067077637</v>
-      </c>
-      <c r="AO2" s="2">
-        <v>32.278564453125</v>
-      </c>
-      <c r="AP2" s="2">
-        <v>12.842391967773438</v>
-      </c>
-      <c r="AQ2" s="2">
-        <v>7.2027759552001953</v>
-      </c>
-      <c r="AR2" s="2">
-        <v>37.126541137695313</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="1">
-        <v>0</v>
+      <c r="AS2" s="2">
+        <v>6.4969592094421387</v>
+      </c>
+      <c r="AT2" s="2">
+        <v>7.8528633117675781</v>
       </c>
       <c r="AU2" s="2">
-        <v>14.665376663208008</v>
+        <v>7.8528633117675781</v>
       </c>
       <c r="AV2" s="2">
-        <v>4.4169931411743164</v>
+        <v>0</v>
       </c>
       <c r="AW2" s="2">
-        <v>3.0003960132598877</v>
+        <v>16.760688781738281</v>
       </c>
       <c r="AX2" s="2">
-        <v>8.2621965408325195</v>
+        <v>31.041105270385742</v>
       </c>
       <c r="AY2" s="2">
-        <v>49.364387512207031</v>
+        <v>2.5635552406311035</v>
       </c>
       <c r="AZ2" s="2">
-        <v>46.937423706054688</v>
+        <v>28.477550506591797</v>
       </c>
       <c r="BA2" s="1">
         <v>0</v>
@@ -629,25 +713,67 @@
         <v>1</v>
       </c>
       <c r="BC2" s="2">
-        <v>1.1367254257202148</v>
+        <v>15.212777137756348</v>
       </c>
       <c r="BD2" s="2">
-        <v>20.284408569335938</v>
+        <v>49.97088623046875</v>
       </c>
       <c r="BE2" s="2">
-        <v>30.025539398193359</v>
+        <v>43.078701019287109</v>
       </c>
       <c r="BF2" s="2">
-        <v>5.3607869148254395</v>
+        <v>6.8921852111816406</v>
       </c>
       <c r="BG2" s="2">
-        <v>34.062877655029297</v>
+        <v>11.978110313415527</v>
       </c>
       <c r="BH2" s="2">
-        <v>37.349773406982422</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>72</v>
+        <v>40.554145812988281</v>
+      </c>
+      <c r="BI2" s="2">
+        <v>4.7253432273864746</v>
+      </c>
+      <c r="BJ2" s="2">
+        <v>35.828804016113281</v>
+      </c>
+      <c r="BK2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM2" s="2">
+        <v>5.5682888031005859</v>
+      </c>
+      <c r="BN2" s="2">
+        <v>5.1995673179626465</v>
+      </c>
+      <c r="BO2" s="2">
+        <v>5.1995673179626465</v>
+      </c>
+      <c r="BP2" s="2">
+        <v>0</v>
+      </c>
+      <c r="BQ2" s="2">
+        <v>5.0970015525817871</v>
+      </c>
+      <c r="BR2" s="2">
+        <v>20.354606628417969</v>
+      </c>
+      <c r="BS2" s="2">
+        <v>14.747118949890137</v>
+      </c>
+      <c r="BT2" s="2">
+        <v>5.607487678527832</v>
+      </c>
+      <c r="BU2" s="1">
+        <v>13.711080551147461</v>
+      </c>
+      <c r="BV2" s="1">
+        <v>1.1302762031555176</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3">
@@ -680,130 +806,130 @@
         <v>2036</v>
       </c>
       <c r="K3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L3" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M3" s="1">
         <v>0</v>
       </c>
       <c r="N3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="2">
-        <v>8.5906248092651367</v>
+        <v>3.1737830638885498</v>
       </c>
       <c r="P3" s="2">
-        <v>14.050758361816406</v>
+        <v>37.302322387695313</v>
       </c>
       <c r="Q3" s="2">
-        <v>12.506132125854492</v>
+        <v>27.001590728759766</v>
       </c>
       <c r="R3" s="2">
-        <v>14.704978942871094</v>
+        <v>10.300731658935547</v>
       </c>
       <c r="S3" s="2">
-        <v>15.732240676879883</v>
+        <v>9.8073272705078125</v>
       </c>
       <c r="T3" s="2">
-        <v>35.372631072998047</v>
-      </c>
-      <c r="U3" s="1">
-        <v>0</v>
-      </c>
-      <c r="V3" s="1">
+        <v>39.558097839355469</v>
+      </c>
+      <c r="U3" s="2">
+        <v>29.271829605102539</v>
+      </c>
+      <c r="V3" s="2">
+        <v>10.28626823425293</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1">
         <v>1</v>
       </c>
-      <c r="W3" s="2">
-        <v>3.9138941764831543</v>
-      </c>
-      <c r="X3" s="2">
-        <v>13.375571250915527</v>
-      </c>
       <c r="Y3" s="2">
-        <v>44.65960693359375</v>
+        <v>16.786825180053711</v>
       </c>
       <c r="Z3" s="2">
-        <v>7.6776456832885742</v>
+        <v>22.355806350708008</v>
       </c>
       <c r="AA3" s="2">
-        <v>38.660953521728516</v>
+        <v>22.355806350708008</v>
       </c>
       <c r="AB3" s="2">
-        <v>30.264581680297852</v>
-      </c>
-      <c r="AC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>16.214475631713867</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>2.23555588722229</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>2.23555588722229</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>9.3099184036254883</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>45.388145446777344</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>34.738975524902344</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>10.649169921875</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>8.2044134140014648</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>33.867767333984375</v>
+      </c>
+      <c r="AO3" s="2">
+        <v>13.838119506835938</v>
+      </c>
+      <c r="AP3" s="2">
+        <v>20.029647827148438</v>
+      </c>
+      <c r="AQ3" s="1">
         <v>1</v>
       </c>
-      <c r="AD3" s="1">
+      <c r="AR3" s="1">
         <v>1</v>
       </c>
-      <c r="AE3" s="2">
-        <v>19.735282897949219</v>
-      </c>
-      <c r="AF3" s="2">
-        <v>39.1041259765625</v>
-      </c>
-      <c r="AG3" s="2">
-        <v>3.3548846244812012</v>
-      </c>
-      <c r="AH3" s="2">
-        <v>4.9948983192443848</v>
-      </c>
-      <c r="AI3" s="2">
-        <v>31.555620193481445</v>
-      </c>
-      <c r="AJ3" s="2">
-        <v>8.9748449325561523</v>
-      </c>
-      <c r="AK3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AM3" s="2">
-        <v>3.3343899250030518</v>
-      </c>
-      <c r="AN3" s="2">
-        <v>12.788989067077637</v>
-      </c>
-      <c r="AO3" s="2">
-        <v>32.278564453125</v>
-      </c>
-      <c r="AP3" s="2">
-        <v>12.842391967773438</v>
-      </c>
-      <c r="AQ3" s="2">
-        <v>7.2027759552001953</v>
-      </c>
-      <c r="AR3" s="2">
-        <v>37.126541137695313</v>
-      </c>
-      <c r="AS3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT3" s="1">
-        <v>0</v>
+      <c r="AS3" s="2">
+        <v>6.4969592094421387</v>
+      </c>
+      <c r="AT3" s="2">
+        <v>7.8528633117675781</v>
       </c>
       <c r="AU3" s="2">
-        <v>14.665376663208008</v>
+        <v>7.8528633117675781</v>
       </c>
       <c r="AV3" s="2">
-        <v>4.4169931411743164</v>
+        <v>0</v>
       </c>
       <c r="AW3" s="2">
-        <v>3.0003960132598877</v>
+        <v>16.760688781738281</v>
       </c>
       <c r="AX3" s="2">
-        <v>8.2621965408325195</v>
+        <v>31.041105270385742</v>
       </c>
       <c r="AY3" s="2">
-        <v>49.364387512207031</v>
+        <v>2.5635552406311035</v>
       </c>
       <c r="AZ3" s="2">
-        <v>46.937423706054688</v>
+        <v>28.477550506591797</v>
       </c>
       <c r="BA3" s="1">
         <v>0</v>
@@ -812,25 +938,67 @@
         <v>1</v>
       </c>
       <c r="BC3" s="2">
-        <v>1.1367254257202148</v>
+        <v>15.212777137756348</v>
       </c>
       <c r="BD3" s="2">
-        <v>20.284408569335938</v>
+        <v>49.97088623046875</v>
       </c>
       <c r="BE3" s="2">
-        <v>30.025539398193359</v>
+        <v>43.078701019287109</v>
       </c>
       <c r="BF3" s="2">
-        <v>5.3607869148254395</v>
+        <v>6.8921852111816406</v>
       </c>
       <c r="BG3" s="2">
-        <v>34.062877655029297</v>
+        <v>11.978110313415527</v>
       </c>
       <c r="BH3" s="2">
-        <v>37.349773406982422</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>72</v>
+        <v>40.554145812988281</v>
+      </c>
+      <c r="BI3" s="2">
+        <v>4.7253432273864746</v>
+      </c>
+      <c r="BJ3" s="2">
+        <v>35.828804016113281</v>
+      </c>
+      <c r="BK3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL3" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM3" s="2">
+        <v>5.5682888031005859</v>
+      </c>
+      <c r="BN3" s="2">
+        <v>5.1995673179626465</v>
+      </c>
+      <c r="BO3" s="2">
+        <v>5.1995673179626465</v>
+      </c>
+      <c r="BP3" s="2">
+        <v>0</v>
+      </c>
+      <c r="BQ3" s="2">
+        <v>5.0970015525817871</v>
+      </c>
+      <c r="BR3" s="2">
+        <v>20.354606628417969</v>
+      </c>
+      <c r="BS3" s="2">
+        <v>14.747118949890137</v>
+      </c>
+      <c r="BT3" s="2">
+        <v>5.607487678527832</v>
+      </c>
+      <c r="BU3" s="1">
+        <v>13.711080551147461</v>
+      </c>
+      <c r="BV3" s="1">
+        <v>1.1302762031555176</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:pencil: Updated session 5 do files
</commit_message>
<xml_diff>
--- a/outputs/03-construccion-datos/duplicates/duplicates.xlsx
+++ b/outputs/03-construccion-datos/duplicates/duplicates.xlsx
@@ -581,40 +581,40 @@
         <v>1978</v>
       </c>
       <c r="K2" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" s="1">
         <v>1</v>
       </c>
       <c r="O2" s="2">
-        <v>3.1737830638885498</v>
+        <v>5.4117140769958496</v>
       </c>
       <c r="P2" s="2">
-        <v>37.302322387695313</v>
+        <v>41.535858154296875</v>
       </c>
       <c r="Q2" s="2">
-        <v>27.001590728759766</v>
+        <v>15.914735794067383</v>
       </c>
       <c r="R2" s="2">
-        <v>10.300731658935547</v>
+        <v>25.621122360229492</v>
       </c>
       <c r="S2" s="2">
-        <v>9.8073272705078125</v>
+        <v>10.464022636413574</v>
       </c>
       <c r="T2" s="2">
-        <v>39.558097839355469</v>
+        <v>37.738624572753906</v>
       </c>
       <c r="U2" s="2">
-        <v>29.271829605102539</v>
+        <v>9.9870309829711914</v>
       </c>
       <c r="V2" s="2">
-        <v>10.28626823425293</v>
+        <v>27.751594543457031</v>
       </c>
       <c r="W2" s="1">
         <v>0</v>
@@ -623,28 +623,28 @@
         <v>1</v>
       </c>
       <c r="Y2" s="2">
-        <v>16.786825180053711</v>
+        <v>6.1416792869567871</v>
       </c>
       <c r="Z2" s="2">
-        <v>22.355806350708008</v>
+        <v>30.753311157226563</v>
       </c>
       <c r="AA2" s="2">
-        <v>22.355806350708008</v>
+        <v>30.753311157226563</v>
       </c>
       <c r="AB2" s="2">
         <v>0</v>
       </c>
       <c r="AC2" s="2">
-        <v>16.214475631713867</v>
+        <v>17.944118499755859</v>
       </c>
       <c r="AD2" s="2">
-        <v>2.23555588722229</v>
+        <v>29.970684051513672</v>
       </c>
       <c r="AE2" s="2">
-        <v>2.23555588722229</v>
+        <v>5.6441683769226074</v>
       </c>
       <c r="AF2" s="2">
-        <v>0</v>
+        <v>24.326515197753906</v>
       </c>
       <c r="AG2" s="1">
         <v>0</v>
@@ -653,28 +653,28 @@
         <v>0</v>
       </c>
       <c r="AI2" s="2">
-        <v>9.3099184036254883</v>
+        <v>10.537778854370117</v>
       </c>
       <c r="AJ2" s="2">
-        <v>45.388145446777344</v>
+        <v>12.444417953491211</v>
       </c>
       <c r="AK2" s="2">
-        <v>34.738975524902344</v>
+        <v>7.4625377655029297</v>
       </c>
       <c r="AL2" s="2">
-        <v>10.649169921875</v>
+        <v>4.9818801879882813</v>
       </c>
       <c r="AM2" s="2">
-        <v>8.2044134140014648</v>
+        <v>19.420539855957031</v>
       </c>
       <c r="AN2" s="2">
-        <v>33.867767333984375</v>
+        <v>34.3587646484375</v>
       </c>
       <c r="AO2" s="2">
-        <v>13.838119506835938</v>
+        <v>23.82172966003418</v>
       </c>
       <c r="AP2" s="2">
-        <v>20.029647827148438</v>
+        <v>10.53703498840332</v>
       </c>
       <c r="AQ2" s="1">
         <v>1</v>
@@ -683,94 +683,94 @@
         <v>1</v>
       </c>
       <c r="AS2" s="2">
-        <v>6.4969592094421387</v>
+        <v>17.804193496704102</v>
       </c>
       <c r="AT2" s="2">
-        <v>7.8528633117675781</v>
+        <v>2.6125538349151611</v>
       </c>
       <c r="AU2" s="2">
-        <v>7.8528633117675781</v>
+        <v>2.6125538349151611</v>
       </c>
       <c r="AV2" s="2">
         <v>0</v>
       </c>
       <c r="AW2" s="2">
-        <v>16.760688781738281</v>
+        <v>2.83695387840271</v>
       </c>
       <c r="AX2" s="2">
-        <v>31.041105270385742</v>
+        <v>31.2218017578125</v>
       </c>
       <c r="AY2" s="2">
-        <v>2.5635552406311035</v>
+        <v>14.377996444702148</v>
       </c>
       <c r="AZ2" s="2">
-        <v>28.477550506591797</v>
+        <v>16.843805313110352</v>
       </c>
       <c r="BA2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC2" s="2">
-        <v>15.212777137756348</v>
+        <v>4.3230438232421875</v>
       </c>
       <c r="BD2" s="2">
-        <v>49.97088623046875</v>
+        <v>9.7958612442016602</v>
       </c>
       <c r="BE2" s="2">
-        <v>43.078701019287109</v>
+        <v>9.7958612442016602</v>
       </c>
       <c r="BF2" s="2">
-        <v>6.8921852111816406</v>
+        <v>0</v>
       </c>
       <c r="BG2" s="2">
-        <v>11.978110313415527</v>
+        <v>13.057753562927246</v>
       </c>
       <c r="BH2" s="2">
-        <v>40.554145812988281</v>
+        <v>5.6126728057861328</v>
       </c>
       <c r="BI2" s="2">
-        <v>4.7253432273864746</v>
+        <v>5.6126728057861328</v>
       </c>
       <c r="BJ2" s="2">
-        <v>35.828804016113281</v>
+        <v>0</v>
       </c>
       <c r="BK2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM2" s="2">
-        <v>5.5682888031005859</v>
+        <v>18.734275817871094</v>
       </c>
       <c r="BN2" s="2">
-        <v>5.1995673179626465</v>
+        <v>9.6759710311889648</v>
       </c>
       <c r="BO2" s="2">
-        <v>5.1995673179626465</v>
+        <v>9.6759710311889648</v>
       </c>
       <c r="BP2" s="2">
         <v>0</v>
       </c>
       <c r="BQ2" s="2">
-        <v>5.0970015525817871</v>
+        <v>14.227289199829102</v>
       </c>
       <c r="BR2" s="2">
-        <v>20.354606628417969</v>
+        <v>34.413803100585938</v>
       </c>
       <c r="BS2" s="2">
-        <v>14.747118949890137</v>
+        <v>20.556005477905273</v>
       </c>
       <c r="BT2" s="2">
-        <v>5.607487678527832</v>
+        <v>13.857797622680664</v>
       </c>
       <c r="BU2" s="1">
-        <v>13.711080551147461</v>
+        <v>2.328934907913208</v>
       </c>
       <c r="BV2" s="1">
-        <v>1.1302762031555176</v>
+        <v>8.7675819396972656</v>
       </c>
       <c r="BW2" t="s">
         <v>86</v>
@@ -806,40 +806,40 @@
         <v>2036</v>
       </c>
       <c r="K3" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="1">
         <v>1</v>
       </c>
       <c r="O3" s="2">
-        <v>3.1737830638885498</v>
+        <v>5.4117140769958496</v>
       </c>
       <c r="P3" s="2">
-        <v>37.302322387695313</v>
+        <v>41.535858154296875</v>
       </c>
       <c r="Q3" s="2">
-        <v>27.001590728759766</v>
+        <v>15.914735794067383</v>
       </c>
       <c r="R3" s="2">
-        <v>10.300731658935547</v>
+        <v>25.621122360229492</v>
       </c>
       <c r="S3" s="2">
-        <v>9.8073272705078125</v>
+        <v>10.464022636413574</v>
       </c>
       <c r="T3" s="2">
-        <v>39.558097839355469</v>
+        <v>37.738624572753906</v>
       </c>
       <c r="U3" s="2">
-        <v>29.271829605102539</v>
+        <v>9.9870309829711914</v>
       </c>
       <c r="V3" s="2">
-        <v>10.28626823425293</v>
+        <v>27.751594543457031</v>
       </c>
       <c r="W3" s="1">
         <v>0</v>
@@ -848,28 +848,28 @@
         <v>1</v>
       </c>
       <c r="Y3" s="2">
-        <v>16.786825180053711</v>
+        <v>6.1416792869567871</v>
       </c>
       <c r="Z3" s="2">
-        <v>22.355806350708008</v>
+        <v>30.753311157226563</v>
       </c>
       <c r="AA3" s="2">
-        <v>22.355806350708008</v>
+        <v>30.753311157226563</v>
       </c>
       <c r="AB3" s="2">
         <v>0</v>
       </c>
       <c r="AC3" s="2">
-        <v>16.214475631713867</v>
+        <v>17.944118499755859</v>
       </c>
       <c r="AD3" s="2">
-        <v>2.23555588722229</v>
+        <v>29.970684051513672</v>
       </c>
       <c r="AE3" s="2">
-        <v>2.23555588722229</v>
+        <v>5.6441683769226074</v>
       </c>
       <c r="AF3" s="2">
-        <v>0</v>
+        <v>24.326515197753906</v>
       </c>
       <c r="AG3" s="1">
         <v>0</v>
@@ -878,28 +878,28 @@
         <v>0</v>
       </c>
       <c r="AI3" s="2">
-        <v>9.3099184036254883</v>
+        <v>10.537778854370117</v>
       </c>
       <c r="AJ3" s="2">
-        <v>45.388145446777344</v>
+        <v>12.444417953491211</v>
       </c>
       <c r="AK3" s="2">
-        <v>34.738975524902344</v>
+        <v>7.4625377655029297</v>
       </c>
       <c r="AL3" s="2">
-        <v>10.649169921875</v>
+        <v>4.9818801879882813</v>
       </c>
       <c r="AM3" s="2">
-        <v>8.2044134140014648</v>
+        <v>19.420539855957031</v>
       </c>
       <c r="AN3" s="2">
-        <v>33.867767333984375</v>
+        <v>34.3587646484375</v>
       </c>
       <c r="AO3" s="2">
-        <v>13.838119506835938</v>
+        <v>23.82172966003418</v>
       </c>
       <c r="AP3" s="2">
-        <v>20.029647827148438</v>
+        <v>10.53703498840332</v>
       </c>
       <c r="AQ3" s="1">
         <v>1</v>
@@ -908,94 +908,94 @@
         <v>1</v>
       </c>
       <c r="AS3" s="2">
-        <v>6.4969592094421387</v>
+        <v>17.804193496704102</v>
       </c>
       <c r="AT3" s="2">
-        <v>7.8528633117675781</v>
+        <v>2.6125538349151611</v>
       </c>
       <c r="AU3" s="2">
-        <v>7.8528633117675781</v>
+        <v>2.6125538349151611</v>
       </c>
       <c r="AV3" s="2">
         <v>0</v>
       </c>
       <c r="AW3" s="2">
-        <v>16.760688781738281</v>
+        <v>2.83695387840271</v>
       </c>
       <c r="AX3" s="2">
-        <v>31.041105270385742</v>
+        <v>31.2218017578125</v>
       </c>
       <c r="AY3" s="2">
-        <v>2.5635552406311035</v>
+        <v>14.377996444702148</v>
       </c>
       <c r="AZ3" s="2">
-        <v>28.477550506591797</v>
+        <v>16.843805313110352</v>
       </c>
       <c r="BA3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC3" s="2">
-        <v>15.212777137756348</v>
+        <v>4.3230438232421875</v>
       </c>
       <c r="BD3" s="2">
-        <v>49.97088623046875</v>
+        <v>9.7958612442016602</v>
       </c>
       <c r="BE3" s="2">
-        <v>43.078701019287109</v>
+        <v>9.7958612442016602</v>
       </c>
       <c r="BF3" s="2">
-        <v>6.8921852111816406</v>
+        <v>0</v>
       </c>
       <c r="BG3" s="2">
-        <v>11.978110313415527</v>
+        <v>13.057753562927246</v>
       </c>
       <c r="BH3" s="2">
-        <v>40.554145812988281</v>
+        <v>5.6126728057861328</v>
       </c>
       <c r="BI3" s="2">
-        <v>4.7253432273864746</v>
+        <v>5.6126728057861328</v>
       </c>
       <c r="BJ3" s="2">
-        <v>35.828804016113281</v>
+        <v>0</v>
       </c>
       <c r="BK3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM3" s="2">
-        <v>5.5682888031005859</v>
+        <v>18.734275817871094</v>
       </c>
       <c r="BN3" s="2">
-        <v>5.1995673179626465</v>
+        <v>9.6759710311889648</v>
       </c>
       <c r="BO3" s="2">
-        <v>5.1995673179626465</v>
+        <v>9.6759710311889648</v>
       </c>
       <c r="BP3" s="2">
         <v>0</v>
       </c>
       <c r="BQ3" s="2">
-        <v>5.0970015525817871</v>
+        <v>14.227289199829102</v>
       </c>
       <c r="BR3" s="2">
-        <v>20.354606628417969</v>
+        <v>34.413803100585938</v>
       </c>
       <c r="BS3" s="2">
-        <v>14.747118949890137</v>
+        <v>20.556005477905273</v>
       </c>
       <c r="BT3" s="2">
-        <v>5.607487678527832</v>
+        <v>13.857797622680664</v>
       </c>
       <c r="BU3" s="1">
-        <v>13.711080551147461</v>
+        <v>2.328934907913208</v>
       </c>
       <c r="BV3" s="1">
-        <v>1.1302762031555176</v>
+        <v>8.7675819396972656</v>
       </c>
       <c r="BW3" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
:pencil: Updated sesion 6 files
</commit_message>
<xml_diff>
--- a/outputs/03-construccion-datos/duplicates/duplicates.xlsx
+++ b/outputs/03-construccion-datos/duplicates/duplicates.xlsx
@@ -584,127 +584,127 @@
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2">
-        <v>5.4117140769958496</v>
+        <v>13.250951766967773</v>
       </c>
       <c r="P2" s="2">
-        <v>41.535858154296875</v>
+        <v>38.024566650390625</v>
       </c>
       <c r="Q2" s="2">
-        <v>15.914735794067383</v>
+        <v>29.036596298217773</v>
       </c>
       <c r="R2" s="2">
-        <v>25.621122360229492</v>
+        <v>8.9879703521728516</v>
       </c>
       <c r="S2" s="2">
-        <v>10.464022636413574</v>
+        <v>3.2160265445709229</v>
       </c>
       <c r="T2" s="2">
-        <v>37.738624572753906</v>
+        <v>35.548210144042969</v>
       </c>
       <c r="U2" s="2">
-        <v>9.9870309829711914</v>
+        <v>8.6075477600097656</v>
       </c>
       <c r="V2" s="2">
-        <v>27.751594543457031</v>
+        <v>26.940662384033203</v>
       </c>
       <c r="W2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="2">
-        <v>6.1416792869567871</v>
+        <v>17.446767807006836</v>
       </c>
       <c r="Z2" s="2">
-        <v>30.753311157226563</v>
+        <v>21.880966186523438</v>
       </c>
       <c r="AA2" s="2">
-        <v>30.753311157226563</v>
+        <v>1.1773288249969482</v>
       </c>
       <c r="AB2" s="2">
-        <v>0</v>
+        <v>20.703638076782227</v>
       </c>
       <c r="AC2" s="2">
-        <v>17.944118499755859</v>
+        <v>8.8961515426635742</v>
       </c>
       <c r="AD2" s="2">
-        <v>29.970684051513672</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AE2" s="2">
-        <v>5.6441683769226074</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AF2" s="2">
-        <v>24.326515197753906</v>
+        <v>0</v>
       </c>
       <c r="AG2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH2" s="1">
         <v>0</v>
       </c>
       <c r="AI2" s="2">
-        <v>10.537778854370117</v>
+        <v>7.0325741767883301</v>
       </c>
       <c r="AJ2" s="2">
-        <v>12.444417953491211</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AK2" s="2">
-        <v>7.4625377655029297</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AL2" s="2">
-        <v>4.9818801879882813</v>
+        <v>0</v>
       </c>
       <c r="AM2" s="2">
-        <v>19.420539855957031</v>
+        <v>4.6432280540466309</v>
       </c>
       <c r="AN2" s="2">
-        <v>34.3587646484375</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AO2" s="2">
-        <v>23.82172966003418</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AP2" s="2">
-        <v>10.53703498840332</v>
+        <v>0</v>
       </c>
       <c r="AQ2" s="1">
         <v>1</v>
       </c>
       <c r="AR2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS2" s="2">
-        <v>17.804193496704102</v>
+        <v>2.3537311553955078</v>
       </c>
       <c r="AT2" s="2">
-        <v>2.6125538349151611</v>
+        <v>32.880050659179688</v>
       </c>
       <c r="AU2" s="2">
-        <v>2.6125538349151611</v>
+        <v>9.2514591217041016</v>
       </c>
       <c r="AV2" s="2">
-        <v>0</v>
+        <v>23.628591537475586</v>
       </c>
       <c r="AW2" s="2">
-        <v>2.83695387840271</v>
+        <v>8.6124334335327148</v>
       </c>
       <c r="AX2" s="2">
-        <v>31.2218017578125</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AY2" s="2">
-        <v>14.377996444702148</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AZ2" s="2">
-        <v>16.843805313110352</v>
+        <v>0</v>
       </c>
       <c r="BA2" s="1">
         <v>1</v>
@@ -713,64 +713,64 @@
         <v>0</v>
       </c>
       <c r="BC2" s="2">
-        <v>4.3230438232421875</v>
+        <v>1.9467545747756958</v>
       </c>
       <c r="BD2" s="2">
-        <v>9.7958612442016602</v>
+        <v>44.056102752685547</v>
       </c>
       <c r="BE2" s="2">
-        <v>9.7958612442016602</v>
+        <v>39.308578491210938</v>
       </c>
       <c r="BF2" s="2">
-        <v>0</v>
+        <v>4.7475242614746094</v>
       </c>
       <c r="BG2" s="2">
-        <v>13.057753562927246</v>
+        <v>3.0712547302246094</v>
       </c>
       <c r="BH2" s="2">
-        <v>5.6126728057861328</v>
+        <v>47.781539916992188</v>
       </c>
       <c r="BI2" s="2">
-        <v>5.6126728057861328</v>
+        <v>43.099933624267578</v>
       </c>
       <c r="BJ2" s="2">
-        <v>0</v>
+        <v>4.6816062927246094</v>
       </c>
       <c r="BK2" s="1">
         <v>1</v>
       </c>
       <c r="BL2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM2" s="2">
-        <v>18.734275817871094</v>
+        <v>18.21574592590332</v>
       </c>
       <c r="BN2" s="2">
-        <v>9.6759710311889648</v>
+        <v>42.9378662109375</v>
       </c>
       <c r="BO2" s="2">
-        <v>9.6759710311889648</v>
+        <v>7.8077750205993652</v>
       </c>
       <c r="BP2" s="2">
-        <v>0</v>
+        <v>35.130092620849609</v>
       </c>
       <c r="BQ2" s="2">
-        <v>14.227289199829102</v>
+        <v>14.384234428405762</v>
       </c>
       <c r="BR2" s="2">
-        <v>34.413803100585938</v>
+        <v>46.834102630615234</v>
       </c>
       <c r="BS2" s="2">
-        <v>20.556005477905273</v>
+        <v>3.9423618316650391</v>
       </c>
       <c r="BT2" s="2">
-        <v>13.857797622680664</v>
+        <v>42.891738891601563</v>
       </c>
       <c r="BU2" s="1">
-        <v>2.328934907913208</v>
+        <v>10.666536331176758</v>
       </c>
       <c r="BV2" s="1">
-        <v>8.7675819396972656</v>
+        <v>7.4639077186584473</v>
       </c>
       <c r="BW2" t="s">
         <v>86</v>
@@ -809,127 +809,127 @@
         <v>0</v>
       </c>
       <c r="L3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="2">
-        <v>5.4117140769958496</v>
+        <v>13.250951766967773</v>
       </c>
       <c r="P3" s="2">
-        <v>41.535858154296875</v>
+        <v>38.024566650390625</v>
       </c>
       <c r="Q3" s="2">
-        <v>15.914735794067383</v>
+        <v>29.036596298217773</v>
       </c>
       <c r="R3" s="2">
-        <v>25.621122360229492</v>
+        <v>8.9879703521728516</v>
       </c>
       <c r="S3" s="2">
-        <v>10.464022636413574</v>
+        <v>3.2160265445709229</v>
       </c>
       <c r="T3" s="2">
-        <v>37.738624572753906</v>
+        <v>35.548210144042969</v>
       </c>
       <c r="U3" s="2">
-        <v>9.9870309829711914</v>
+        <v>8.6075477600097656</v>
       </c>
       <c r="V3" s="2">
-        <v>27.751594543457031</v>
+        <v>26.940662384033203</v>
       </c>
       <c r="W3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="2">
-        <v>6.1416792869567871</v>
+        <v>17.446767807006836</v>
       </c>
       <c r="Z3" s="2">
-        <v>30.753311157226563</v>
+        <v>21.880966186523438</v>
       </c>
       <c r="AA3" s="2">
-        <v>30.753311157226563</v>
+        <v>1.1773288249969482</v>
       </c>
       <c r="AB3" s="2">
-        <v>0</v>
+        <v>20.703638076782227</v>
       </c>
       <c r="AC3" s="2">
-        <v>17.944118499755859</v>
+        <v>8.8961515426635742</v>
       </c>
       <c r="AD3" s="2">
-        <v>29.970684051513672</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AE3" s="2">
-        <v>5.6441683769226074</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AF3" s="2">
-        <v>24.326515197753906</v>
+        <v>0</v>
       </c>
       <c r="AG3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH3" s="1">
         <v>0</v>
       </c>
       <c r="AI3" s="2">
-        <v>10.537778854370117</v>
+        <v>7.0325741767883301</v>
       </c>
       <c r="AJ3" s="2">
-        <v>12.444417953491211</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AK3" s="2">
-        <v>7.4625377655029297</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AL3" s="2">
-        <v>4.9818801879882813</v>
+        <v>0</v>
       </c>
       <c r="AM3" s="2">
-        <v>19.420539855957031</v>
+        <v>4.6432280540466309</v>
       </c>
       <c r="AN3" s="2">
-        <v>34.3587646484375</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AO3" s="2">
-        <v>23.82172966003418</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AP3" s="2">
-        <v>10.53703498840332</v>
+        <v>0</v>
       </c>
       <c r="AQ3" s="1">
         <v>1</v>
       </c>
       <c r="AR3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS3" s="2">
-        <v>17.804193496704102</v>
+        <v>2.3537311553955078</v>
       </c>
       <c r="AT3" s="2">
-        <v>2.6125538349151611</v>
+        <v>32.880050659179688</v>
       </c>
       <c r="AU3" s="2">
-        <v>2.6125538349151611</v>
+        <v>9.2514591217041016</v>
       </c>
       <c r="AV3" s="2">
-        <v>0</v>
+        <v>23.628591537475586</v>
       </c>
       <c r="AW3" s="2">
-        <v>2.83695387840271</v>
+        <v>8.6124334335327148</v>
       </c>
       <c r="AX3" s="2">
-        <v>31.2218017578125</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AY3" s="2">
-        <v>14.377996444702148</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AZ3" s="2">
-        <v>16.843805313110352</v>
+        <v>0</v>
       </c>
       <c r="BA3" s="1">
         <v>1</v>
@@ -938,64 +938,64 @@
         <v>0</v>
       </c>
       <c r="BC3" s="2">
-        <v>4.3230438232421875</v>
+        <v>1.9467545747756958</v>
       </c>
       <c r="BD3" s="2">
-        <v>9.7958612442016602</v>
+        <v>44.056102752685547</v>
       </c>
       <c r="BE3" s="2">
-        <v>9.7958612442016602</v>
+        <v>39.308578491210938</v>
       </c>
       <c r="BF3" s="2">
-        <v>0</v>
+        <v>4.7475242614746094</v>
       </c>
       <c r="BG3" s="2">
-        <v>13.057753562927246</v>
+        <v>3.0712547302246094</v>
       </c>
       <c r="BH3" s="2">
-        <v>5.6126728057861328</v>
+        <v>47.781539916992188</v>
       </c>
       <c r="BI3" s="2">
-        <v>5.6126728057861328</v>
+        <v>43.099933624267578</v>
       </c>
       <c r="BJ3" s="2">
-        <v>0</v>
+        <v>4.6816062927246094</v>
       </c>
       <c r="BK3" s="1">
         <v>1</v>
       </c>
       <c r="BL3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM3" s="2">
-        <v>18.734275817871094</v>
+        <v>18.21574592590332</v>
       </c>
       <c r="BN3" s="2">
-        <v>9.6759710311889648</v>
+        <v>42.9378662109375</v>
       </c>
       <c r="BO3" s="2">
-        <v>9.6759710311889648</v>
+        <v>7.8077750205993652</v>
       </c>
       <c r="BP3" s="2">
-        <v>0</v>
+        <v>35.130092620849609</v>
       </c>
       <c r="BQ3" s="2">
-        <v>14.227289199829102</v>
+        <v>14.384234428405762</v>
       </c>
       <c r="BR3" s="2">
-        <v>34.413803100585938</v>
+        <v>46.834102630615234</v>
       </c>
       <c r="BS3" s="2">
-        <v>20.556005477905273</v>
+        <v>3.9423618316650391</v>
       </c>
       <c r="BT3" s="2">
-        <v>13.857797622680664</v>
+        <v>42.891738891601563</v>
       </c>
       <c r="BU3" s="1">
-        <v>2.328934907913208</v>
+        <v>10.666536331176758</v>
       </c>
       <c r="BV3" s="1">
-        <v>8.7675819396972656</v>
+        <v>7.4639077186584473</v>
       </c>
       <c r="BW3" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
:pencil: Updated sesion 8 files and fixed old do files
</commit_message>
<xml_diff>
--- a/outputs/03-construccion-datos/duplicates/duplicates.xlsx
+++ b/outputs/03-construccion-datos/duplicates/duplicates.xlsx
@@ -581,10 +581,10 @@
         <v>1978</v>
       </c>
       <c r="K2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
@@ -593,148 +593,148 @@
         <v>0</v>
       </c>
       <c r="O2" s="2">
-        <v>13.250951766967773</v>
+        <v>5.7680816650390625</v>
       </c>
       <c r="P2" s="2">
-        <v>38.024566650390625</v>
+        <v>2.2352011203765869</v>
       </c>
       <c r="Q2" s="2">
-        <v>29.036596298217773</v>
+        <v>2.2352011203765869</v>
       </c>
       <c r="R2" s="2">
-        <v>8.9879703521728516</v>
+        <v>0</v>
       </c>
       <c r="S2" s="2">
-        <v>3.2160265445709229</v>
+        <v>19.658470153808594</v>
       </c>
       <c r="T2" s="2">
-        <v>35.548210144042969</v>
+        <v>42.728260040283203</v>
       </c>
       <c r="U2" s="2">
-        <v>8.6075477600097656</v>
+        <v>40.030673980712891</v>
       </c>
       <c r="V2" s="2">
-        <v>26.940662384033203</v>
+        <v>2.6975860595703125</v>
       </c>
       <c r="W2" s="1">
         <v>1</v>
       </c>
       <c r="X2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="2">
-        <v>17.446767807006836</v>
+        <v>16.939168930053711</v>
       </c>
       <c r="Z2" s="2">
-        <v>21.880966186523438</v>
+        <v>16.453506469726563</v>
       </c>
       <c r="AA2" s="2">
-        <v>1.1773288249969482</v>
+        <v>16.453506469726563</v>
       </c>
       <c r="AB2" s="2">
-        <v>20.703638076782227</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="2">
-        <v>8.8961515426635742</v>
+        <v>14.110039710998535</v>
       </c>
       <c r="AD2" s="2">
-        <v>2.1978754997253418</v>
+        <v>34.581287384033203</v>
       </c>
       <c r="AE2" s="2">
-        <v>2.1978754997253418</v>
+        <v>7.0867562294006348</v>
       </c>
       <c r="AF2" s="2">
-        <v>0</v>
+        <v>27.494531631469727</v>
       </c>
       <c r="AG2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH2" s="1">
         <v>0</v>
       </c>
       <c r="AI2" s="2">
-        <v>7.0325741767883301</v>
+        <v>4.0451245307922363</v>
       </c>
       <c r="AJ2" s="2">
-        <v>29.231773376464844</v>
+        <v>17.451549530029297</v>
       </c>
       <c r="AK2" s="2">
-        <v>29.231773376464844</v>
+        <v>17.451549530029297</v>
       </c>
       <c r="AL2" s="2">
         <v>0</v>
       </c>
       <c r="AM2" s="2">
-        <v>4.6432280540466309</v>
+        <v>2.4514777660369873</v>
       </c>
       <c r="AN2" s="2">
-        <v>8.4582910537719727</v>
+        <v>44.512004852294922</v>
       </c>
       <c r="AO2" s="2">
-        <v>8.4582910537719727</v>
+        <v>17.808340072631836</v>
       </c>
       <c r="AP2" s="2">
-        <v>0</v>
+        <v>26.703664779663086</v>
       </c>
       <c r="AQ2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR2" s="1">
         <v>0</v>
       </c>
       <c r="AS2" s="2">
-        <v>2.3537311553955078</v>
+        <v>3.6109740734100342</v>
       </c>
       <c r="AT2" s="2">
-        <v>32.880050659179688</v>
+        <v>27.876899719238281</v>
       </c>
       <c r="AU2" s="2">
-        <v>9.2514591217041016</v>
+        <v>20.809535980224609</v>
       </c>
       <c r="AV2" s="2">
-        <v>23.628591537475586</v>
+        <v>7.0673637390136719</v>
       </c>
       <c r="AW2" s="2">
-        <v>8.6124334335327148</v>
+        <v>9.8803443908691406</v>
       </c>
       <c r="AX2" s="2">
-        <v>13.234278678894043</v>
+        <v>8.5362758636474609</v>
       </c>
       <c r="AY2" s="2">
-        <v>13.234278678894043</v>
+        <v>8.5362758636474609</v>
       </c>
       <c r="AZ2" s="2">
         <v>0</v>
       </c>
       <c r="BA2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB2" s="1">
         <v>0</v>
       </c>
       <c r="BC2" s="2">
-        <v>1.9467545747756958</v>
+        <v>3.2463028430938721</v>
       </c>
       <c r="BD2" s="2">
-        <v>44.056102752685547</v>
+        <v>32.966930389404297</v>
       </c>
       <c r="BE2" s="2">
-        <v>39.308578491210938</v>
+        <v>32.966930389404297</v>
       </c>
       <c r="BF2" s="2">
-        <v>4.7475242614746094</v>
+        <v>0</v>
       </c>
       <c r="BG2" s="2">
-        <v>3.0712547302246094</v>
+        <v>8.0707817077636719</v>
       </c>
       <c r="BH2" s="2">
-        <v>47.781539916992188</v>
+        <v>11.795376777648926</v>
       </c>
       <c r="BI2" s="2">
-        <v>43.099933624267578</v>
+        <v>11.795376777648926</v>
       </c>
       <c r="BJ2" s="2">
-        <v>4.6816062927246094</v>
+        <v>0</v>
       </c>
       <c r="BK2" s="1">
         <v>1</v>
@@ -743,34 +743,34 @@
         <v>0</v>
       </c>
       <c r="BM2" s="2">
-        <v>18.21574592590332</v>
+        <v>5.4777421951293945</v>
       </c>
       <c r="BN2" s="2">
-        <v>42.9378662109375</v>
+        <v>44.768749237060547</v>
       </c>
       <c r="BO2" s="2">
-        <v>7.8077750205993652</v>
+        <v>5.536811351776123</v>
       </c>
       <c r="BP2" s="2">
-        <v>35.130092620849609</v>
+        <v>39.231937408447266</v>
       </c>
       <c r="BQ2" s="2">
-        <v>14.384234428405762</v>
+        <v>1.8907539844512939</v>
       </c>
       <c r="BR2" s="2">
-        <v>46.834102630615234</v>
+        <v>6.6376943588256836</v>
       </c>
       <c r="BS2" s="2">
-        <v>3.9423618316650391</v>
+        <v>3.558706521987915</v>
       </c>
       <c r="BT2" s="2">
-        <v>42.891738891601563</v>
+        <v>3.0789878368377686</v>
       </c>
       <c r="BU2" s="1">
-        <v>10.666536331176758</v>
+        <v>10.387241363525391</v>
       </c>
       <c r="BV2" s="1">
-        <v>7.4639077186584473</v>
+        <v>7.8235669136047363</v>
       </c>
       <c r="BW2" t="s">
         <v>86</v>
@@ -806,10 +806,10 @@
         <v>2036</v>
       </c>
       <c r="K3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M3" s="1">
         <v>0</v>
@@ -818,148 +818,148 @@
         <v>0</v>
       </c>
       <c r="O3" s="2">
-        <v>13.250951766967773</v>
+        <v>5.7680816650390625</v>
       </c>
       <c r="P3" s="2">
-        <v>38.024566650390625</v>
+        <v>2.2352011203765869</v>
       </c>
       <c r="Q3" s="2">
-        <v>29.036596298217773</v>
+        <v>2.2352011203765869</v>
       </c>
       <c r="R3" s="2">
-        <v>8.9879703521728516</v>
+        <v>0</v>
       </c>
       <c r="S3" s="2">
-        <v>3.2160265445709229</v>
+        <v>19.658470153808594</v>
       </c>
       <c r="T3" s="2">
-        <v>35.548210144042969</v>
+        <v>42.728260040283203</v>
       </c>
       <c r="U3" s="2">
-        <v>8.6075477600097656</v>
+        <v>40.030673980712891</v>
       </c>
       <c r="V3" s="2">
-        <v>26.940662384033203</v>
+        <v>2.6975860595703125</v>
       </c>
       <c r="W3" s="1">
         <v>1</v>
       </c>
       <c r="X3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3" s="2">
-        <v>17.446767807006836</v>
+        <v>16.939168930053711</v>
       </c>
       <c r="Z3" s="2">
-        <v>21.880966186523438</v>
+        <v>16.453506469726563</v>
       </c>
       <c r="AA3" s="2">
-        <v>1.1773288249969482</v>
+        <v>16.453506469726563</v>
       </c>
       <c r="AB3" s="2">
-        <v>20.703638076782227</v>
+        <v>0</v>
       </c>
       <c r="AC3" s="2">
-        <v>8.8961515426635742</v>
+        <v>14.110039710998535</v>
       </c>
       <c r="AD3" s="2">
-        <v>2.1978754997253418</v>
+        <v>34.581287384033203</v>
       </c>
       <c r="AE3" s="2">
-        <v>2.1978754997253418</v>
+        <v>7.0867562294006348</v>
       </c>
       <c r="AF3" s="2">
-        <v>0</v>
+        <v>27.494531631469727</v>
       </c>
       <c r="AG3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH3" s="1">
         <v>0</v>
       </c>
       <c r="AI3" s="2">
-        <v>7.0325741767883301</v>
+        <v>4.0451245307922363</v>
       </c>
       <c r="AJ3" s="2">
-        <v>29.231773376464844</v>
+        <v>17.451549530029297</v>
       </c>
       <c r="AK3" s="2">
-        <v>29.231773376464844</v>
+        <v>17.451549530029297</v>
       </c>
       <c r="AL3" s="2">
         <v>0</v>
       </c>
       <c r="AM3" s="2">
-        <v>4.6432280540466309</v>
+        <v>2.4514777660369873</v>
       </c>
       <c r="AN3" s="2">
-        <v>8.4582910537719727</v>
+        <v>44.512004852294922</v>
       </c>
       <c r="AO3" s="2">
-        <v>8.4582910537719727</v>
+        <v>17.808340072631836</v>
       </c>
       <c r="AP3" s="2">
-        <v>0</v>
+        <v>26.703664779663086</v>
       </c>
       <c r="AQ3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR3" s="1">
         <v>0</v>
       </c>
       <c r="AS3" s="2">
-        <v>2.3537311553955078</v>
+        <v>3.6109740734100342</v>
       </c>
       <c r="AT3" s="2">
-        <v>32.880050659179688</v>
+        <v>27.876899719238281</v>
       </c>
       <c r="AU3" s="2">
-        <v>9.2514591217041016</v>
+        <v>20.809535980224609</v>
       </c>
       <c r="AV3" s="2">
-        <v>23.628591537475586</v>
+        <v>7.0673637390136719</v>
       </c>
       <c r="AW3" s="2">
-        <v>8.6124334335327148</v>
+        <v>9.8803443908691406</v>
       </c>
       <c r="AX3" s="2">
-        <v>13.234278678894043</v>
+        <v>8.5362758636474609</v>
       </c>
       <c r="AY3" s="2">
-        <v>13.234278678894043</v>
+        <v>8.5362758636474609</v>
       </c>
       <c r="AZ3" s="2">
         <v>0</v>
       </c>
       <c r="BA3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB3" s="1">
         <v>0</v>
       </c>
       <c r="BC3" s="2">
-        <v>1.9467545747756958</v>
+        <v>3.2463028430938721</v>
       </c>
       <c r="BD3" s="2">
-        <v>44.056102752685547</v>
+        <v>32.966930389404297</v>
       </c>
       <c r="BE3" s="2">
-        <v>39.308578491210938</v>
+        <v>32.966930389404297</v>
       </c>
       <c r="BF3" s="2">
-        <v>4.7475242614746094</v>
+        <v>0</v>
       </c>
       <c r="BG3" s="2">
-        <v>3.0712547302246094</v>
+        <v>8.0707817077636719</v>
       </c>
       <c r="BH3" s="2">
-        <v>47.781539916992188</v>
+        <v>11.795376777648926</v>
       </c>
       <c r="BI3" s="2">
-        <v>43.099933624267578</v>
+        <v>11.795376777648926</v>
       </c>
       <c r="BJ3" s="2">
-        <v>4.6816062927246094</v>
+        <v>0</v>
       </c>
       <c r="BK3" s="1">
         <v>1</v>
@@ -968,34 +968,34 @@
         <v>0</v>
       </c>
       <c r="BM3" s="2">
-        <v>18.21574592590332</v>
+        <v>5.4777421951293945</v>
       </c>
       <c r="BN3" s="2">
-        <v>42.9378662109375</v>
+        <v>44.768749237060547</v>
       </c>
       <c r="BO3" s="2">
-        <v>7.8077750205993652</v>
+        <v>5.536811351776123</v>
       </c>
       <c r="BP3" s="2">
-        <v>35.130092620849609</v>
+        <v>39.231937408447266</v>
       </c>
       <c r="BQ3" s="2">
-        <v>14.384234428405762</v>
+        <v>1.8907539844512939</v>
       </c>
       <c r="BR3" s="2">
-        <v>46.834102630615234</v>
+        <v>6.6376943588256836</v>
       </c>
       <c r="BS3" s="2">
-        <v>3.9423618316650391</v>
+        <v>3.558706521987915</v>
       </c>
       <c r="BT3" s="2">
-        <v>42.891738891601563</v>
+        <v>3.0789878368377686</v>
       </c>
       <c r="BU3" s="1">
-        <v>10.666536331176758</v>
+        <v>10.387241363525391</v>
       </c>
       <c r="BV3" s="1">
-        <v>7.4639077186584473</v>
+        <v>7.8235669136047363</v>
       </c>
       <c r="BW3" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
:pencil: actualizado minor text diff en la sesion 3 do files
</commit_message>
<xml_diff>
--- a/outputs/03-construccion-datos/duplicates/duplicates.xlsx
+++ b/outputs/03-construccion-datos/duplicates/duplicates.xlsx
@@ -24,7 +24,7 @@
     <t>datelisted</t>
   </si>
   <si>
-    <t>12Jul2020</t>
+    <t>23Jan2021</t>
   </si>
   <si>
     <t>datefixed</t>
@@ -581,196 +581,196 @@
         <v>1978</v>
       </c>
       <c r="K2" s="1">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
+        <v>5.4615616798400879</v>
+      </c>
+      <c r="P2" s="2">
+        <v>36.344417572021484</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>15.732240676879883</v>
+      </c>
+      <c r="R2" s="2">
+        <v>20.612176895141602</v>
+      </c>
+      <c r="S2" s="2">
+        <v>14.328163146972656</v>
+      </c>
+      <c r="T2" s="2">
+        <v>9.2889471054077148</v>
+      </c>
+      <c r="U2" s="2">
+        <v>9.2889471054077148</v>
+      </c>
+      <c r="V2" s="2">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>17.929235458374023</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>18.221296310424805</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>18.221296310424805</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>12.347491264343262</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>41.844860076904297</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>29.519598007202148</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>12.325262069702148</v>
+      </c>
+      <c r="AG2" s="1">
         <v>1</v>
       </c>
-      <c r="L2" s="1">
-        <v>5</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2">
-        <v>5.7680816650390625</v>
-      </c>
-      <c r="P2" s="2">
-        <v>2.2352011203765869</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>2.2352011203765869</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2">
-        <v>19.658470153808594</v>
-      </c>
-      <c r="T2" s="2">
-        <v>42.728260040283203</v>
-      </c>
-      <c r="U2" s="2">
-        <v>40.030673980712891</v>
-      </c>
-      <c r="V2" s="2">
-        <v>2.6975860595703125</v>
-      </c>
-      <c r="W2" s="1">
+      <c r="AH2" s="1">
         <v>1</v>
       </c>
-      <c r="X2" s="1">
+      <c r="AI2" s="2">
+        <v>1.9131186008453369</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>11.302633285522461</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>11.302633285522461</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>4.0922870635986328</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>39.660980224609375</v>
+      </c>
+      <c r="AO2" s="2">
+        <v>39.660980224609375</v>
+      </c>
+      <c r="AP2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="2">
+        <v>13.128422737121582</v>
+      </c>
+      <c r="AT2" s="2">
+        <v>31.540904998779297</v>
+      </c>
+      <c r="AU2" s="2">
+        <v>7.2027759552001953</v>
+      </c>
+      <c r="AV2" s="2">
+        <v>24.338129043579102</v>
+      </c>
+      <c r="AW2" s="2">
+        <v>15.00825023651123</v>
+      </c>
+      <c r="AX2" s="2">
+        <v>41.836856842041016</v>
+      </c>
+      <c r="AY2" s="2">
+        <v>23.532167434692383</v>
+      </c>
+      <c r="AZ2" s="2">
+        <v>18.304689407348633</v>
+      </c>
+      <c r="BA2" s="1">
         <v>1</v>
       </c>
-      <c r="Y2" s="2">
-        <v>16.939168930053711</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>16.453506469726563</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>16.453506469726563</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>14.110039710998535</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>34.581287384033203</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>7.0867562294006348</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>27.494531631469727</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>4.0451245307922363</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>17.451549530029297</v>
-      </c>
-      <c r="AK2" s="2">
-        <v>17.451549530029297</v>
-      </c>
-      <c r="AL2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="2">
-        <v>2.4514777660369873</v>
-      </c>
-      <c r="AN2" s="2">
-        <v>44.512004852294922</v>
-      </c>
-      <c r="AO2" s="2">
-        <v>17.808340072631836</v>
-      </c>
-      <c r="AP2" s="2">
-        <v>26.703664779663086</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="2">
-        <v>3.6109740734100342</v>
-      </c>
-      <c r="AT2" s="2">
-        <v>27.876899719238281</v>
-      </c>
-      <c r="AU2" s="2">
-        <v>20.809535980224609</v>
-      </c>
-      <c r="AV2" s="2">
-        <v>7.0673637390136719</v>
-      </c>
-      <c r="AW2" s="2">
-        <v>9.8803443908691406</v>
-      </c>
-      <c r="AX2" s="2">
-        <v>8.5362758636474609</v>
-      </c>
-      <c r="AY2" s="2">
-        <v>8.5362758636474609</v>
-      </c>
-      <c r="AZ2" s="2">
-        <v>0</v>
-      </c>
-      <c r="BA2" s="1">
-        <v>0</v>
-      </c>
       <c r="BB2" s="1">
         <v>0</v>
       </c>
       <c r="BC2" s="2">
-        <v>3.2463028430938721</v>
+        <v>1.7756637334823608</v>
       </c>
       <c r="BD2" s="2">
-        <v>32.966930389404297</v>
+        <v>19.728822708129883</v>
       </c>
       <c r="BE2" s="2">
-        <v>32.966930389404297</v>
+        <v>19.728822708129883</v>
       </c>
       <c r="BF2" s="2">
         <v>0</v>
       </c>
       <c r="BG2" s="2">
-        <v>8.0707817077636719</v>
+        <v>18.812471389770508</v>
       </c>
       <c r="BH2" s="2">
-        <v>11.795376777648926</v>
+        <v>13.198483467102051</v>
       </c>
       <c r="BI2" s="2">
-        <v>11.795376777648926</v>
+        <v>13.198483467102051</v>
       </c>
       <c r="BJ2" s="2">
         <v>0</v>
       </c>
       <c r="BK2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL2" s="1">
         <v>0</v>
       </c>
       <c r="BM2" s="2">
-        <v>5.4777421951293945</v>
+        <v>12.254801750183105</v>
       </c>
       <c r="BN2" s="2">
-        <v>44.768749237060547</v>
+        <v>12.24623966217041</v>
       </c>
       <c r="BO2" s="2">
-        <v>5.536811351776123</v>
+        <v>12.24623966217041</v>
       </c>
       <c r="BP2" s="2">
-        <v>39.231937408447266</v>
+        <v>0</v>
       </c>
       <c r="BQ2" s="2">
-        <v>1.8907539844512939</v>
+        <v>15.094810485839844</v>
       </c>
       <c r="BR2" s="2">
-        <v>6.6376943588256836</v>
+        <v>34.425300598144531</v>
       </c>
       <c r="BS2" s="2">
-        <v>3.558706521987915</v>
+        <v>32.867267608642578</v>
       </c>
       <c r="BT2" s="2">
-        <v>3.0789878368377686</v>
+        <v>1.5580329895019531</v>
       </c>
       <c r="BU2" s="1">
-        <v>10.387241363525391</v>
+        <v>4.588139533996582</v>
       </c>
       <c r="BV2" s="1">
-        <v>7.8235669136047363</v>
+        <v>8.8507347106933594</v>
       </c>
       <c r="BW2" t="s">
         <v>86</v>
@@ -806,196 +806,196 @@
         <v>2036</v>
       </c>
       <c r="K3" s="1">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1">
+        <v>6</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>5.4615616798400879</v>
+      </c>
+      <c r="P3" s="2">
+        <v>36.344417572021484</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>15.732240676879883</v>
+      </c>
+      <c r="R3" s="2">
+        <v>20.612176895141602</v>
+      </c>
+      <c r="S3" s="2">
+        <v>14.328163146972656</v>
+      </c>
+      <c r="T3" s="2">
+        <v>9.2889471054077148</v>
+      </c>
+      <c r="U3" s="2">
+        <v>9.2889471054077148</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>17.929235458374023</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>18.221296310424805</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>18.221296310424805</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>12.347491264343262</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>41.844860076904297</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>29.519598007202148</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>12.325262069702148</v>
+      </c>
+      <c r="AG3" s="1">
         <v>1</v>
       </c>
-      <c r="L3" s="1">
-        <v>5</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>5.7680816650390625</v>
-      </c>
-      <c r="P3" s="2">
-        <v>2.2352011203765869</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>2.2352011203765869</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0</v>
-      </c>
-      <c r="S3" s="2">
-        <v>19.658470153808594</v>
-      </c>
-      <c r="T3" s="2">
-        <v>42.728260040283203</v>
-      </c>
-      <c r="U3" s="2">
-        <v>40.030673980712891</v>
-      </c>
-      <c r="V3" s="2">
-        <v>2.6975860595703125</v>
-      </c>
-      <c r="W3" s="1">
+      <c r="AH3" s="1">
         <v>1</v>
       </c>
-      <c r="X3" s="1">
+      <c r="AI3" s="2">
+        <v>1.9131186008453369</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>11.302633285522461</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>11.302633285522461</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>4.0922870635986328</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>39.660980224609375</v>
+      </c>
+      <c r="AO3" s="2">
+        <v>39.660980224609375</v>
+      </c>
+      <c r="AP3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="2">
+        <v>13.128422737121582</v>
+      </c>
+      <c r="AT3" s="2">
+        <v>31.540904998779297</v>
+      </c>
+      <c r="AU3" s="2">
+        <v>7.2027759552001953</v>
+      </c>
+      <c r="AV3" s="2">
+        <v>24.338129043579102</v>
+      </c>
+      <c r="AW3" s="2">
+        <v>15.00825023651123</v>
+      </c>
+      <c r="AX3" s="2">
+        <v>41.836856842041016</v>
+      </c>
+      <c r="AY3" s="2">
+        <v>23.532167434692383</v>
+      </c>
+      <c r="AZ3" s="2">
+        <v>18.304689407348633</v>
+      </c>
+      <c r="BA3" s="1">
         <v>1</v>
       </c>
-      <c r="Y3" s="2">
-        <v>16.939168930053711</v>
-      </c>
-      <c r="Z3" s="2">
-        <v>16.453506469726563</v>
-      </c>
-      <c r="AA3" s="2">
-        <v>16.453506469726563</v>
-      </c>
-      <c r="AB3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="2">
-        <v>14.110039710998535</v>
-      </c>
-      <c r="AD3" s="2">
-        <v>34.581287384033203</v>
-      </c>
-      <c r="AE3" s="2">
-        <v>7.0867562294006348</v>
-      </c>
-      <c r="AF3" s="2">
-        <v>27.494531631469727</v>
-      </c>
-      <c r="AG3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="2">
-        <v>4.0451245307922363</v>
-      </c>
-      <c r="AJ3" s="2">
-        <v>17.451549530029297</v>
-      </c>
-      <c r="AK3" s="2">
-        <v>17.451549530029297</v>
-      </c>
-      <c r="AL3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="2">
-        <v>2.4514777660369873</v>
-      </c>
-      <c r="AN3" s="2">
-        <v>44.512004852294922</v>
-      </c>
-      <c r="AO3" s="2">
-        <v>17.808340072631836</v>
-      </c>
-      <c r="AP3" s="2">
-        <v>26.703664779663086</v>
-      </c>
-      <c r="AQ3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="2">
-        <v>3.6109740734100342</v>
-      </c>
-      <c r="AT3" s="2">
-        <v>27.876899719238281</v>
-      </c>
-      <c r="AU3" s="2">
-        <v>20.809535980224609</v>
-      </c>
-      <c r="AV3" s="2">
-        <v>7.0673637390136719</v>
-      </c>
-      <c r="AW3" s="2">
-        <v>9.8803443908691406</v>
-      </c>
-      <c r="AX3" s="2">
-        <v>8.5362758636474609</v>
-      </c>
-      <c r="AY3" s="2">
-        <v>8.5362758636474609</v>
-      </c>
-      <c r="AZ3" s="2">
-        <v>0</v>
-      </c>
-      <c r="BA3" s="1">
-        <v>0</v>
-      </c>
       <c r="BB3" s="1">
         <v>0</v>
       </c>
       <c r="BC3" s="2">
-        <v>3.2463028430938721</v>
+        <v>1.7756637334823608</v>
       </c>
       <c r="BD3" s="2">
-        <v>32.966930389404297</v>
+        <v>19.728822708129883</v>
       </c>
       <c r="BE3" s="2">
-        <v>32.966930389404297</v>
+        <v>19.728822708129883</v>
       </c>
       <c r="BF3" s="2">
         <v>0</v>
       </c>
       <c r="BG3" s="2">
-        <v>8.0707817077636719</v>
+        <v>18.812471389770508</v>
       </c>
       <c r="BH3" s="2">
-        <v>11.795376777648926</v>
+        <v>13.198483467102051</v>
       </c>
       <c r="BI3" s="2">
-        <v>11.795376777648926</v>
+        <v>13.198483467102051</v>
       </c>
       <c r="BJ3" s="2">
         <v>0</v>
       </c>
       <c r="BK3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL3" s="1">
         <v>0</v>
       </c>
       <c r="BM3" s="2">
-        <v>5.4777421951293945</v>
+        <v>12.254801750183105</v>
       </c>
       <c r="BN3" s="2">
-        <v>44.768749237060547</v>
+        <v>12.24623966217041</v>
       </c>
       <c r="BO3" s="2">
-        <v>5.536811351776123</v>
+        <v>12.24623966217041</v>
       </c>
       <c r="BP3" s="2">
-        <v>39.231937408447266</v>
+        <v>0</v>
       </c>
       <c r="BQ3" s="2">
-        <v>1.8907539844512939</v>
+        <v>15.094810485839844</v>
       </c>
       <c r="BR3" s="2">
-        <v>6.6376943588256836</v>
+        <v>34.425300598144531</v>
       </c>
       <c r="BS3" s="2">
-        <v>3.558706521987915</v>
+        <v>32.867267608642578</v>
       </c>
       <c r="BT3" s="2">
-        <v>3.0789878368377686</v>
+        <v>1.5580329895019531</v>
       </c>
       <c r="BU3" s="1">
-        <v>10.387241363525391</v>
+        <v>4.588139533996582</v>
       </c>
       <c r="BV3" s="1">
-        <v>7.8235669136047363</v>
+        <v>8.8507347106933594</v>
       </c>
       <c r="BW3" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
:pencil: cambios a do file y slides de la sesión 5
</commit_message>
<xml_diff>
--- a/outputs/03-construccion-datos/duplicates/duplicates.xlsx
+++ b/outputs/03-construccion-datos/duplicates/duplicates.xlsx
@@ -581,10 +581,10 @@
         <v>1978</v>
       </c>
       <c r="K2" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
@@ -593,118 +593,118 @@
         <v>0</v>
       </c>
       <c r="O2" s="2">
-        <v>5.4615616798400879</v>
+        <v>13.250951766967773</v>
       </c>
       <c r="P2" s="2">
-        <v>36.344417572021484</v>
+        <v>38.024566650390625</v>
       </c>
       <c r="Q2" s="2">
-        <v>15.732240676879883</v>
+        <v>29.036596298217773</v>
       </c>
       <c r="R2" s="2">
-        <v>20.612176895141602</v>
+        <v>8.9879703521728516</v>
       </c>
       <c r="S2" s="2">
-        <v>14.328163146972656</v>
+        <v>3.2160265445709229</v>
       </c>
       <c r="T2" s="2">
-        <v>9.2889471054077148</v>
+        <v>35.548210144042969</v>
       </c>
       <c r="U2" s="2">
-        <v>9.2889471054077148</v>
+        <v>8.6075477600097656</v>
       </c>
       <c r="V2" s="2">
-        <v>0</v>
+        <v>26.940662384033203</v>
       </c>
       <c r="W2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2" s="1">
         <v>0</v>
       </c>
       <c r="Y2" s="2">
-        <v>17.929235458374023</v>
+        <v>17.446767807006836</v>
       </c>
       <c r="Z2" s="2">
-        <v>18.221296310424805</v>
+        <v>21.880966186523438</v>
       </c>
       <c r="AA2" s="2">
-        <v>18.221296310424805</v>
+        <v>1.1773288249969482</v>
       </c>
       <c r="AB2" s="2">
-        <v>0</v>
+        <v>20.703638076782227</v>
       </c>
       <c r="AC2" s="2">
-        <v>12.347491264343262</v>
+        <v>8.8961515426635742</v>
       </c>
       <c r="AD2" s="2">
-        <v>41.844860076904297</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AE2" s="2">
-        <v>29.519598007202148</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AF2" s="2">
-        <v>12.325262069702148</v>
+        <v>0</v>
       </c>
       <c r="AG2" s="1">
         <v>1</v>
       </c>
       <c r="AH2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI2" s="2">
-        <v>1.9131186008453369</v>
+        <v>7.0325741767883301</v>
       </c>
       <c r="AJ2" s="2">
-        <v>11.302633285522461</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AK2" s="2">
-        <v>11.302633285522461</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AL2" s="2">
         <v>0</v>
       </c>
       <c r="AM2" s="2">
-        <v>4.0922870635986328</v>
+        <v>4.6432280540466309</v>
       </c>
       <c r="AN2" s="2">
-        <v>39.660980224609375</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AO2" s="2">
-        <v>39.660980224609375</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AP2" s="2">
         <v>0</v>
       </c>
       <c r="AQ2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR2" s="1">
         <v>0</v>
       </c>
       <c r="AS2" s="2">
-        <v>13.128422737121582</v>
+        <v>2.3537311553955078</v>
       </c>
       <c r="AT2" s="2">
-        <v>31.540904998779297</v>
+        <v>32.880050659179688</v>
       </c>
       <c r="AU2" s="2">
-        <v>7.2027759552001953</v>
+        <v>9.2514591217041016</v>
       </c>
       <c r="AV2" s="2">
-        <v>24.338129043579102</v>
+        <v>23.628591537475586</v>
       </c>
       <c r="AW2" s="2">
-        <v>15.00825023651123</v>
+        <v>8.6124334335327148</v>
       </c>
       <c r="AX2" s="2">
-        <v>41.836856842041016</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AY2" s="2">
-        <v>23.532167434692383</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AZ2" s="2">
-        <v>18.304689407348633</v>
+        <v>0</v>
       </c>
       <c r="BA2" s="1">
         <v>1</v>
@@ -713,64 +713,64 @@
         <v>0</v>
       </c>
       <c r="BC2" s="2">
-        <v>1.7756637334823608</v>
+        <v>1.9467545747756958</v>
       </c>
       <c r="BD2" s="2">
-        <v>19.728822708129883</v>
+        <v>44.056102752685547</v>
       </c>
       <c r="BE2" s="2">
-        <v>19.728822708129883</v>
+        <v>39.308578491210938</v>
       </c>
       <c r="BF2" s="2">
-        <v>0</v>
+        <v>4.7475242614746094</v>
       </c>
       <c r="BG2" s="2">
-        <v>18.812471389770508</v>
+        <v>3.0712547302246094</v>
       </c>
       <c r="BH2" s="2">
-        <v>13.198483467102051</v>
+        <v>47.781539916992188</v>
       </c>
       <c r="BI2" s="2">
-        <v>13.198483467102051</v>
+        <v>43.099933624267578</v>
       </c>
       <c r="BJ2" s="2">
-        <v>0</v>
+        <v>4.6816062927246094</v>
       </c>
       <c r="BK2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL2" s="1">
         <v>0</v>
       </c>
       <c r="BM2" s="2">
-        <v>12.254801750183105</v>
+        <v>18.21574592590332</v>
       </c>
       <c r="BN2" s="2">
-        <v>12.24623966217041</v>
+        <v>42.9378662109375</v>
       </c>
       <c r="BO2" s="2">
-        <v>12.24623966217041</v>
+        <v>7.8077750205993652</v>
       </c>
       <c r="BP2" s="2">
-        <v>0</v>
+        <v>35.130092620849609</v>
       </c>
       <c r="BQ2" s="2">
-        <v>15.094810485839844</v>
+        <v>14.384234428405762</v>
       </c>
       <c r="BR2" s="2">
-        <v>34.425300598144531</v>
+        <v>46.834102630615234</v>
       </c>
       <c r="BS2" s="2">
-        <v>32.867267608642578</v>
+        <v>3.9423618316650391</v>
       </c>
       <c r="BT2" s="2">
-        <v>1.5580329895019531</v>
+        <v>42.891738891601563</v>
       </c>
       <c r="BU2" s="1">
-        <v>4.588139533996582</v>
+        <v>10.666536331176758</v>
       </c>
       <c r="BV2" s="1">
-        <v>8.8507347106933594</v>
+        <v>7.4639077186584473</v>
       </c>
       <c r="BW2" t="s">
         <v>86</v>
@@ -806,10 +806,10 @@
         <v>2036</v>
       </c>
       <c r="K3" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M3" s="1">
         <v>0</v>
@@ -818,118 +818,118 @@
         <v>0</v>
       </c>
       <c r="O3" s="2">
-        <v>5.4615616798400879</v>
+        <v>13.250951766967773</v>
       </c>
       <c r="P3" s="2">
-        <v>36.344417572021484</v>
+        <v>38.024566650390625</v>
       </c>
       <c r="Q3" s="2">
-        <v>15.732240676879883</v>
+        <v>29.036596298217773</v>
       </c>
       <c r="R3" s="2">
-        <v>20.612176895141602</v>
+        <v>8.9879703521728516</v>
       </c>
       <c r="S3" s="2">
-        <v>14.328163146972656</v>
+        <v>3.2160265445709229</v>
       </c>
       <c r="T3" s="2">
-        <v>9.2889471054077148</v>
+        <v>35.548210144042969</v>
       </c>
       <c r="U3" s="2">
-        <v>9.2889471054077148</v>
+        <v>8.6075477600097656</v>
       </c>
       <c r="V3" s="2">
-        <v>0</v>
+        <v>26.940662384033203</v>
       </c>
       <c r="W3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3" s="1">
         <v>0</v>
       </c>
       <c r="Y3" s="2">
-        <v>17.929235458374023</v>
+        <v>17.446767807006836</v>
       </c>
       <c r="Z3" s="2">
-        <v>18.221296310424805</v>
+        <v>21.880966186523438</v>
       </c>
       <c r="AA3" s="2">
-        <v>18.221296310424805</v>
+        <v>1.1773288249969482</v>
       </c>
       <c r="AB3" s="2">
-        <v>0</v>
+        <v>20.703638076782227</v>
       </c>
       <c r="AC3" s="2">
-        <v>12.347491264343262</v>
+        <v>8.8961515426635742</v>
       </c>
       <c r="AD3" s="2">
-        <v>41.844860076904297</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AE3" s="2">
-        <v>29.519598007202148</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AF3" s="2">
-        <v>12.325262069702148</v>
+        <v>0</v>
       </c>
       <c r="AG3" s="1">
         <v>1</v>
       </c>
       <c r="AH3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI3" s="2">
-        <v>1.9131186008453369</v>
+        <v>7.0325741767883301</v>
       </c>
       <c r="AJ3" s="2">
-        <v>11.302633285522461</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AK3" s="2">
-        <v>11.302633285522461</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AL3" s="2">
         <v>0</v>
       </c>
       <c r="AM3" s="2">
-        <v>4.0922870635986328</v>
+        <v>4.6432280540466309</v>
       </c>
       <c r="AN3" s="2">
-        <v>39.660980224609375</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AO3" s="2">
-        <v>39.660980224609375</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AP3" s="2">
         <v>0</v>
       </c>
       <c r="AQ3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR3" s="1">
         <v>0</v>
       </c>
       <c r="AS3" s="2">
-        <v>13.128422737121582</v>
+        <v>2.3537311553955078</v>
       </c>
       <c r="AT3" s="2">
-        <v>31.540904998779297</v>
+        <v>32.880050659179688</v>
       </c>
       <c r="AU3" s="2">
-        <v>7.2027759552001953</v>
+        <v>9.2514591217041016</v>
       </c>
       <c r="AV3" s="2">
-        <v>24.338129043579102</v>
+        <v>23.628591537475586</v>
       </c>
       <c r="AW3" s="2">
-        <v>15.00825023651123</v>
+        <v>8.6124334335327148</v>
       </c>
       <c r="AX3" s="2">
-        <v>41.836856842041016</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AY3" s="2">
-        <v>23.532167434692383</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AZ3" s="2">
-        <v>18.304689407348633</v>
+        <v>0</v>
       </c>
       <c r="BA3" s="1">
         <v>1</v>
@@ -938,64 +938,64 @@
         <v>0</v>
       </c>
       <c r="BC3" s="2">
-        <v>1.7756637334823608</v>
+        <v>1.9467545747756958</v>
       </c>
       <c r="BD3" s="2">
-        <v>19.728822708129883</v>
+        <v>44.056102752685547</v>
       </c>
       <c r="BE3" s="2">
-        <v>19.728822708129883</v>
+        <v>39.308578491210938</v>
       </c>
       <c r="BF3" s="2">
-        <v>0</v>
+        <v>4.7475242614746094</v>
       </c>
       <c r="BG3" s="2">
-        <v>18.812471389770508</v>
+        <v>3.0712547302246094</v>
       </c>
       <c r="BH3" s="2">
-        <v>13.198483467102051</v>
+        <v>47.781539916992188</v>
       </c>
       <c r="BI3" s="2">
-        <v>13.198483467102051</v>
+        <v>43.099933624267578</v>
       </c>
       <c r="BJ3" s="2">
-        <v>0</v>
+        <v>4.6816062927246094</v>
       </c>
       <c r="BK3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL3" s="1">
         <v>0</v>
       </c>
       <c r="BM3" s="2">
-        <v>12.254801750183105</v>
+        <v>18.21574592590332</v>
       </c>
       <c r="BN3" s="2">
-        <v>12.24623966217041</v>
+        <v>42.9378662109375</v>
       </c>
       <c r="BO3" s="2">
-        <v>12.24623966217041</v>
+        <v>7.8077750205993652</v>
       </c>
       <c r="BP3" s="2">
-        <v>0</v>
+        <v>35.130092620849609</v>
       </c>
       <c r="BQ3" s="2">
-        <v>15.094810485839844</v>
+        <v>14.384234428405762</v>
       </c>
       <c r="BR3" s="2">
-        <v>34.425300598144531</v>
+        <v>46.834102630615234</v>
       </c>
       <c r="BS3" s="2">
-        <v>32.867267608642578</v>
+        <v>3.9423618316650391</v>
       </c>
       <c r="BT3" s="2">
-        <v>1.5580329895019531</v>
+        <v>42.891738891601563</v>
       </c>
       <c r="BU3" s="1">
-        <v>4.588139533996582</v>
+        <v>10.666536331176758</v>
       </c>
       <c r="BV3" s="1">
-        <v>8.8507347106933594</v>
+        <v>7.4639077186584473</v>
       </c>
       <c r="BW3" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
:pencil: cambios a dofile sesion 5 de la semana 3
</commit_message>
<xml_diff>
--- a/outputs/03-construccion-datos/duplicates/duplicates.xlsx
+++ b/outputs/03-construccion-datos/duplicates/duplicates.xlsx
@@ -584,127 +584,127 @@
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" s="2">
-        <v>13.250951766967773</v>
+        <v>5.4117140769958496</v>
       </c>
       <c r="P2" s="2">
-        <v>38.024566650390625</v>
+        <v>41.535858154296875</v>
       </c>
       <c r="Q2" s="2">
-        <v>29.036596298217773</v>
+        <v>15.914735794067383</v>
       </c>
       <c r="R2" s="2">
-        <v>8.9879703521728516</v>
+        <v>25.621122360229492</v>
       </c>
       <c r="S2" s="2">
-        <v>3.2160265445709229</v>
+        <v>10.464022636413574</v>
       </c>
       <c r="T2" s="2">
-        <v>35.548210144042969</v>
+        <v>37.738624572753906</v>
       </c>
       <c r="U2" s="2">
-        <v>8.6075477600097656</v>
+        <v>9.9870309829711914</v>
       </c>
       <c r="V2" s="2">
-        <v>26.940662384033203</v>
+        <v>27.751594543457031</v>
       </c>
       <c r="W2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="2">
-        <v>17.446767807006836</v>
+        <v>6.1416792869567871</v>
       </c>
       <c r="Z2" s="2">
-        <v>21.880966186523438</v>
+        <v>30.753311157226563</v>
       </c>
       <c r="AA2" s="2">
-        <v>1.1773288249969482</v>
+        <v>30.753311157226563</v>
       </c>
       <c r="AB2" s="2">
-        <v>20.703638076782227</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="2">
-        <v>8.8961515426635742</v>
+        <v>17.944118499755859</v>
       </c>
       <c r="AD2" s="2">
-        <v>2.1978754997253418</v>
+        <v>29.970684051513672</v>
       </c>
       <c r="AE2" s="2">
-        <v>2.1978754997253418</v>
+        <v>5.6441683769226074</v>
       </c>
       <c r="AF2" s="2">
-        <v>0</v>
+        <v>24.326515197753906</v>
       </c>
       <c r="AG2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH2" s="1">
         <v>0</v>
       </c>
       <c r="AI2" s="2">
-        <v>7.0325741767883301</v>
+        <v>10.537778854370117</v>
       </c>
       <c r="AJ2" s="2">
-        <v>29.231773376464844</v>
+        <v>12.444417953491211</v>
       </c>
       <c r="AK2" s="2">
-        <v>29.231773376464844</v>
+        <v>7.4625377655029297</v>
       </c>
       <c r="AL2" s="2">
-        <v>0</v>
+        <v>4.9818801879882813</v>
       </c>
       <c r="AM2" s="2">
-        <v>4.6432280540466309</v>
+        <v>19.420539855957031</v>
       </c>
       <c r="AN2" s="2">
-        <v>8.4582910537719727</v>
+        <v>34.3587646484375</v>
       </c>
       <c r="AO2" s="2">
-        <v>8.4582910537719727</v>
+        <v>23.82172966003418</v>
       </c>
       <c r="AP2" s="2">
-        <v>0</v>
+        <v>10.53703498840332</v>
       </c>
       <c r="AQ2" s="1">
         <v>1</v>
       </c>
       <c r="AR2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS2" s="2">
-        <v>2.3537311553955078</v>
+        <v>17.804193496704102</v>
       </c>
       <c r="AT2" s="2">
-        <v>32.880050659179688</v>
+        <v>2.6125538349151611</v>
       </c>
       <c r="AU2" s="2">
-        <v>9.2514591217041016</v>
+        <v>2.6125538349151611</v>
       </c>
       <c r="AV2" s="2">
-        <v>23.628591537475586</v>
+        <v>0</v>
       </c>
       <c r="AW2" s="2">
-        <v>8.6124334335327148</v>
+        <v>2.83695387840271</v>
       </c>
       <c r="AX2" s="2">
-        <v>13.234278678894043</v>
+        <v>31.2218017578125</v>
       </c>
       <c r="AY2" s="2">
-        <v>13.234278678894043</v>
+        <v>14.377996444702148</v>
       </c>
       <c r="AZ2" s="2">
-        <v>0</v>
+        <v>16.843805313110352</v>
       </c>
       <c r="BA2" s="1">
         <v>1</v>
@@ -713,64 +713,64 @@
         <v>0</v>
       </c>
       <c r="BC2" s="2">
-        <v>1.9467545747756958</v>
+        <v>4.3230438232421875</v>
       </c>
       <c r="BD2" s="2">
-        <v>44.056102752685547</v>
+        <v>9.7958612442016602</v>
       </c>
       <c r="BE2" s="2">
-        <v>39.308578491210938</v>
+        <v>9.7958612442016602</v>
       </c>
       <c r="BF2" s="2">
-        <v>4.7475242614746094</v>
+        <v>0</v>
       </c>
       <c r="BG2" s="2">
-        <v>3.0712547302246094</v>
+        <v>13.057753562927246</v>
       </c>
       <c r="BH2" s="2">
-        <v>47.781539916992188</v>
+        <v>5.6126728057861328</v>
       </c>
       <c r="BI2" s="2">
-        <v>43.099933624267578</v>
+        <v>5.6126728057861328</v>
       </c>
       <c r="BJ2" s="2">
-        <v>4.6816062927246094</v>
+        <v>0</v>
       </c>
       <c r="BK2" s="1">
         <v>1</v>
       </c>
       <c r="BL2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM2" s="2">
-        <v>18.21574592590332</v>
+        <v>18.734275817871094</v>
       </c>
       <c r="BN2" s="2">
-        <v>42.9378662109375</v>
+        <v>9.6759710311889648</v>
       </c>
       <c r="BO2" s="2">
-        <v>7.8077750205993652</v>
+        <v>9.6759710311889648</v>
       </c>
       <c r="BP2" s="2">
-        <v>35.130092620849609</v>
+        <v>0</v>
       </c>
       <c r="BQ2" s="2">
-        <v>14.384234428405762</v>
+        <v>14.227289199829102</v>
       </c>
       <c r="BR2" s="2">
-        <v>46.834102630615234</v>
+        <v>34.413803100585938</v>
       </c>
       <c r="BS2" s="2">
-        <v>3.9423618316650391</v>
+        <v>20.556005477905273</v>
       </c>
       <c r="BT2" s="2">
-        <v>42.891738891601563</v>
+        <v>13.857797622680664</v>
       </c>
       <c r="BU2" s="1">
-        <v>10.666536331176758</v>
+        <v>2.328934907913208</v>
       </c>
       <c r="BV2" s="1">
-        <v>7.4639077186584473</v>
+        <v>8.7675819396972656</v>
       </c>
       <c r="BW2" t="s">
         <v>86</v>
@@ -809,127 +809,127 @@
         <v>0</v>
       </c>
       <c r="L3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="2">
-        <v>13.250951766967773</v>
+        <v>5.4117140769958496</v>
       </c>
       <c r="P3" s="2">
-        <v>38.024566650390625</v>
+        <v>41.535858154296875</v>
       </c>
       <c r="Q3" s="2">
-        <v>29.036596298217773</v>
+        <v>15.914735794067383</v>
       </c>
       <c r="R3" s="2">
-        <v>8.9879703521728516</v>
+        <v>25.621122360229492</v>
       </c>
       <c r="S3" s="2">
-        <v>3.2160265445709229</v>
+        <v>10.464022636413574</v>
       </c>
       <c r="T3" s="2">
-        <v>35.548210144042969</v>
+        <v>37.738624572753906</v>
       </c>
       <c r="U3" s="2">
-        <v>8.6075477600097656</v>
+        <v>9.9870309829711914</v>
       </c>
       <c r="V3" s="2">
-        <v>26.940662384033203</v>
+        <v>27.751594543457031</v>
       </c>
       <c r="W3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3" s="2">
-        <v>17.446767807006836</v>
+        <v>6.1416792869567871</v>
       </c>
       <c r="Z3" s="2">
-        <v>21.880966186523438</v>
+        <v>30.753311157226563</v>
       </c>
       <c r="AA3" s="2">
-        <v>1.1773288249969482</v>
+        <v>30.753311157226563</v>
       </c>
       <c r="AB3" s="2">
-        <v>20.703638076782227</v>
+        <v>0</v>
       </c>
       <c r="AC3" s="2">
-        <v>8.8961515426635742</v>
+        <v>17.944118499755859</v>
       </c>
       <c r="AD3" s="2">
-        <v>2.1978754997253418</v>
+        <v>29.970684051513672</v>
       </c>
       <c r="AE3" s="2">
-        <v>2.1978754997253418</v>
+        <v>5.6441683769226074</v>
       </c>
       <c r="AF3" s="2">
-        <v>0</v>
+        <v>24.326515197753906</v>
       </c>
       <c r="AG3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH3" s="1">
         <v>0</v>
       </c>
       <c r="AI3" s="2">
-        <v>7.0325741767883301</v>
+        <v>10.537778854370117</v>
       </c>
       <c r="AJ3" s="2">
-        <v>29.231773376464844</v>
+        <v>12.444417953491211</v>
       </c>
       <c r="AK3" s="2">
-        <v>29.231773376464844</v>
+        <v>7.4625377655029297</v>
       </c>
       <c r="AL3" s="2">
-        <v>0</v>
+        <v>4.9818801879882813</v>
       </c>
       <c r="AM3" s="2">
-        <v>4.6432280540466309</v>
+        <v>19.420539855957031</v>
       </c>
       <c r="AN3" s="2">
-        <v>8.4582910537719727</v>
+        <v>34.3587646484375</v>
       </c>
       <c r="AO3" s="2">
-        <v>8.4582910537719727</v>
+        <v>23.82172966003418</v>
       </c>
       <c r="AP3" s="2">
-        <v>0</v>
+        <v>10.53703498840332</v>
       </c>
       <c r="AQ3" s="1">
         <v>1</v>
       </c>
       <c r="AR3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS3" s="2">
-        <v>2.3537311553955078</v>
+        <v>17.804193496704102</v>
       </c>
       <c r="AT3" s="2">
-        <v>32.880050659179688</v>
+        <v>2.6125538349151611</v>
       </c>
       <c r="AU3" s="2">
-        <v>9.2514591217041016</v>
+        <v>2.6125538349151611</v>
       </c>
       <c r="AV3" s="2">
-        <v>23.628591537475586</v>
+        <v>0</v>
       </c>
       <c r="AW3" s="2">
-        <v>8.6124334335327148</v>
+        <v>2.83695387840271</v>
       </c>
       <c r="AX3" s="2">
-        <v>13.234278678894043</v>
+        <v>31.2218017578125</v>
       </c>
       <c r="AY3" s="2">
-        <v>13.234278678894043</v>
+        <v>14.377996444702148</v>
       </c>
       <c r="AZ3" s="2">
-        <v>0</v>
+        <v>16.843805313110352</v>
       </c>
       <c r="BA3" s="1">
         <v>1</v>
@@ -938,64 +938,64 @@
         <v>0</v>
       </c>
       <c r="BC3" s="2">
-        <v>1.9467545747756958</v>
+        <v>4.3230438232421875</v>
       </c>
       <c r="BD3" s="2">
-        <v>44.056102752685547</v>
+        <v>9.7958612442016602</v>
       </c>
       <c r="BE3" s="2">
-        <v>39.308578491210938</v>
+        <v>9.7958612442016602</v>
       </c>
       <c r="BF3" s="2">
-        <v>4.7475242614746094</v>
+        <v>0</v>
       </c>
       <c r="BG3" s="2">
-        <v>3.0712547302246094</v>
+        <v>13.057753562927246</v>
       </c>
       <c r="BH3" s="2">
-        <v>47.781539916992188</v>
+        <v>5.6126728057861328</v>
       </c>
       <c r="BI3" s="2">
-        <v>43.099933624267578</v>
+        <v>5.6126728057861328</v>
       </c>
       <c r="BJ3" s="2">
-        <v>4.6816062927246094</v>
+        <v>0</v>
       </c>
       <c r="BK3" s="1">
         <v>1</v>
       </c>
       <c r="BL3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM3" s="2">
-        <v>18.21574592590332</v>
+        <v>18.734275817871094</v>
       </c>
       <c r="BN3" s="2">
-        <v>42.9378662109375</v>
+        <v>9.6759710311889648</v>
       </c>
       <c r="BO3" s="2">
-        <v>7.8077750205993652</v>
+        <v>9.6759710311889648</v>
       </c>
       <c r="BP3" s="2">
-        <v>35.130092620849609</v>
+        <v>0</v>
       </c>
       <c r="BQ3" s="2">
-        <v>14.384234428405762</v>
+        <v>14.227289199829102</v>
       </c>
       <c r="BR3" s="2">
-        <v>46.834102630615234</v>
+        <v>34.413803100585938</v>
       </c>
       <c r="BS3" s="2">
-        <v>3.9423618316650391</v>
+        <v>20.556005477905273</v>
       </c>
       <c r="BT3" s="2">
-        <v>42.891738891601563</v>
+        <v>13.857797622680664</v>
       </c>
       <c r="BU3" s="1">
-        <v>10.666536331176758</v>
+        <v>2.328934907913208</v>
       </c>
       <c r="BV3" s="1">
-        <v>7.4639077186584473</v>
+        <v>8.7675819396972656</v>
       </c>
       <c r="BW3" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
:pencil: cambios a do file sesion 6 de la semana 3
</commit_message>
<xml_diff>
--- a/outputs/03-construccion-datos/duplicates/duplicates.xlsx
+++ b/outputs/03-construccion-datos/duplicates/duplicates.xlsx
@@ -584,127 +584,127 @@
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2">
-        <v>5.4117140769958496</v>
+        <v>13.250951766967773</v>
       </c>
       <c r="P2" s="2">
-        <v>41.535858154296875</v>
+        <v>38.024566650390625</v>
       </c>
       <c r="Q2" s="2">
-        <v>15.914735794067383</v>
+        <v>29.036596298217773</v>
       </c>
       <c r="R2" s="2">
-        <v>25.621122360229492</v>
+        <v>8.9879703521728516</v>
       </c>
       <c r="S2" s="2">
-        <v>10.464022636413574</v>
+        <v>3.2160265445709229</v>
       </c>
       <c r="T2" s="2">
-        <v>37.738624572753906</v>
+        <v>35.548210144042969</v>
       </c>
       <c r="U2" s="2">
-        <v>9.9870309829711914</v>
+        <v>8.6075477600097656</v>
       </c>
       <c r="V2" s="2">
-        <v>27.751594543457031</v>
+        <v>26.940662384033203</v>
       </c>
       <c r="W2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="2">
-        <v>6.1416792869567871</v>
+        <v>17.446767807006836</v>
       </c>
       <c r="Z2" s="2">
-        <v>30.753311157226563</v>
+        <v>21.880966186523438</v>
       </c>
       <c r="AA2" s="2">
-        <v>30.753311157226563</v>
+        <v>1.1773288249969482</v>
       </c>
       <c r="AB2" s="2">
-        <v>0</v>
+        <v>20.703638076782227</v>
       </c>
       <c r="AC2" s="2">
-        <v>17.944118499755859</v>
+        <v>8.8961515426635742</v>
       </c>
       <c r="AD2" s="2">
-        <v>29.970684051513672</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AE2" s="2">
-        <v>5.6441683769226074</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AF2" s="2">
-        <v>24.326515197753906</v>
+        <v>0</v>
       </c>
       <c r="AG2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH2" s="1">
         <v>0</v>
       </c>
       <c r="AI2" s="2">
-        <v>10.537778854370117</v>
+        <v>7.0325741767883301</v>
       </c>
       <c r="AJ2" s="2">
-        <v>12.444417953491211</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AK2" s="2">
-        <v>7.4625377655029297</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AL2" s="2">
-        <v>4.9818801879882813</v>
+        <v>0</v>
       </c>
       <c r="AM2" s="2">
-        <v>19.420539855957031</v>
+        <v>4.6432280540466309</v>
       </c>
       <c r="AN2" s="2">
-        <v>34.3587646484375</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AO2" s="2">
-        <v>23.82172966003418</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AP2" s="2">
-        <v>10.53703498840332</v>
+        <v>0</v>
       </c>
       <c r="AQ2" s="1">
         <v>1</v>
       </c>
       <c r="AR2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS2" s="2">
-        <v>17.804193496704102</v>
+        <v>2.3537311553955078</v>
       </c>
       <c r="AT2" s="2">
-        <v>2.6125538349151611</v>
+        <v>32.880050659179688</v>
       </c>
       <c r="AU2" s="2">
-        <v>2.6125538349151611</v>
+        <v>9.2514591217041016</v>
       </c>
       <c r="AV2" s="2">
-        <v>0</v>
+        <v>23.628591537475586</v>
       </c>
       <c r="AW2" s="2">
-        <v>2.83695387840271</v>
+        <v>8.6124334335327148</v>
       </c>
       <c r="AX2" s="2">
-        <v>31.2218017578125</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AY2" s="2">
-        <v>14.377996444702148</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AZ2" s="2">
-        <v>16.843805313110352</v>
+        <v>0</v>
       </c>
       <c r="BA2" s="1">
         <v>1</v>
@@ -713,64 +713,64 @@
         <v>0</v>
       </c>
       <c r="BC2" s="2">
-        <v>4.3230438232421875</v>
+        <v>1.9467545747756958</v>
       </c>
       <c r="BD2" s="2">
-        <v>9.7958612442016602</v>
+        <v>44.056102752685547</v>
       </c>
       <c r="BE2" s="2">
-        <v>9.7958612442016602</v>
+        <v>39.308578491210938</v>
       </c>
       <c r="BF2" s="2">
-        <v>0</v>
+        <v>4.7475242614746094</v>
       </c>
       <c r="BG2" s="2">
-        <v>13.057753562927246</v>
+        <v>3.0712547302246094</v>
       </c>
       <c r="BH2" s="2">
-        <v>5.6126728057861328</v>
+        <v>47.781539916992188</v>
       </c>
       <c r="BI2" s="2">
-        <v>5.6126728057861328</v>
+        <v>43.099933624267578</v>
       </c>
       <c r="BJ2" s="2">
-        <v>0</v>
+        <v>4.6816062927246094</v>
       </c>
       <c r="BK2" s="1">
         <v>1</v>
       </c>
       <c r="BL2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM2" s="2">
-        <v>18.734275817871094</v>
+        <v>18.21574592590332</v>
       </c>
       <c r="BN2" s="2">
-        <v>9.6759710311889648</v>
+        <v>42.9378662109375</v>
       </c>
       <c r="BO2" s="2">
-        <v>9.6759710311889648</v>
+        <v>7.8077750205993652</v>
       </c>
       <c r="BP2" s="2">
-        <v>0</v>
+        <v>35.130092620849609</v>
       </c>
       <c r="BQ2" s="2">
-        <v>14.227289199829102</v>
+        <v>14.384234428405762</v>
       </c>
       <c r="BR2" s="2">
-        <v>34.413803100585938</v>
+        <v>46.834102630615234</v>
       </c>
       <c r="BS2" s="2">
-        <v>20.556005477905273</v>
+        <v>3.9423618316650391</v>
       </c>
       <c r="BT2" s="2">
-        <v>13.857797622680664</v>
+        <v>42.891738891601563</v>
       </c>
       <c r="BU2" s="1">
-        <v>2.328934907913208</v>
+        <v>10.666536331176758</v>
       </c>
       <c r="BV2" s="1">
-        <v>8.7675819396972656</v>
+        <v>7.4639077186584473</v>
       </c>
       <c r="BW2" t="s">
         <v>86</v>
@@ -809,127 +809,127 @@
         <v>0</v>
       </c>
       <c r="L3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="2">
-        <v>5.4117140769958496</v>
+        <v>13.250951766967773</v>
       </c>
       <c r="P3" s="2">
-        <v>41.535858154296875</v>
+        <v>38.024566650390625</v>
       </c>
       <c r="Q3" s="2">
-        <v>15.914735794067383</v>
+        <v>29.036596298217773</v>
       </c>
       <c r="R3" s="2">
-        <v>25.621122360229492</v>
+        <v>8.9879703521728516</v>
       </c>
       <c r="S3" s="2">
-        <v>10.464022636413574</v>
+        <v>3.2160265445709229</v>
       </c>
       <c r="T3" s="2">
-        <v>37.738624572753906</v>
+        <v>35.548210144042969</v>
       </c>
       <c r="U3" s="2">
-        <v>9.9870309829711914</v>
+        <v>8.6075477600097656</v>
       </c>
       <c r="V3" s="2">
-        <v>27.751594543457031</v>
+        <v>26.940662384033203</v>
       </c>
       <c r="W3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="2">
-        <v>6.1416792869567871</v>
+        <v>17.446767807006836</v>
       </c>
       <c r="Z3" s="2">
-        <v>30.753311157226563</v>
+        <v>21.880966186523438</v>
       </c>
       <c r="AA3" s="2">
-        <v>30.753311157226563</v>
+        <v>1.1773288249969482</v>
       </c>
       <c r="AB3" s="2">
-        <v>0</v>
+        <v>20.703638076782227</v>
       </c>
       <c r="AC3" s="2">
-        <v>17.944118499755859</v>
+        <v>8.8961515426635742</v>
       </c>
       <c r="AD3" s="2">
-        <v>29.970684051513672</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AE3" s="2">
-        <v>5.6441683769226074</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AF3" s="2">
-        <v>24.326515197753906</v>
+        <v>0</v>
       </c>
       <c r="AG3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH3" s="1">
         <v>0</v>
       </c>
       <c r="AI3" s="2">
-        <v>10.537778854370117</v>
+        <v>7.0325741767883301</v>
       </c>
       <c r="AJ3" s="2">
-        <v>12.444417953491211</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AK3" s="2">
-        <v>7.4625377655029297</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AL3" s="2">
-        <v>4.9818801879882813</v>
+        <v>0</v>
       </c>
       <c r="AM3" s="2">
-        <v>19.420539855957031</v>
+        <v>4.6432280540466309</v>
       </c>
       <c r="AN3" s="2">
-        <v>34.3587646484375</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AO3" s="2">
-        <v>23.82172966003418</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AP3" s="2">
-        <v>10.53703498840332</v>
+        <v>0</v>
       </c>
       <c r="AQ3" s="1">
         <v>1</v>
       </c>
       <c r="AR3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS3" s="2">
-        <v>17.804193496704102</v>
+        <v>2.3537311553955078</v>
       </c>
       <c r="AT3" s="2">
-        <v>2.6125538349151611</v>
+        <v>32.880050659179688</v>
       </c>
       <c r="AU3" s="2">
-        <v>2.6125538349151611</v>
+        <v>9.2514591217041016</v>
       </c>
       <c r="AV3" s="2">
-        <v>0</v>
+        <v>23.628591537475586</v>
       </c>
       <c r="AW3" s="2">
-        <v>2.83695387840271</v>
+        <v>8.6124334335327148</v>
       </c>
       <c r="AX3" s="2">
-        <v>31.2218017578125</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AY3" s="2">
-        <v>14.377996444702148</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AZ3" s="2">
-        <v>16.843805313110352</v>
+        <v>0</v>
       </c>
       <c r="BA3" s="1">
         <v>1</v>
@@ -938,64 +938,64 @@
         <v>0</v>
       </c>
       <c r="BC3" s="2">
-        <v>4.3230438232421875</v>
+        <v>1.9467545747756958</v>
       </c>
       <c r="BD3" s="2">
-        <v>9.7958612442016602</v>
+        <v>44.056102752685547</v>
       </c>
       <c r="BE3" s="2">
-        <v>9.7958612442016602</v>
+        <v>39.308578491210938</v>
       </c>
       <c r="BF3" s="2">
-        <v>0</v>
+        <v>4.7475242614746094</v>
       </c>
       <c r="BG3" s="2">
-        <v>13.057753562927246</v>
+        <v>3.0712547302246094</v>
       </c>
       <c r="BH3" s="2">
-        <v>5.6126728057861328</v>
+        <v>47.781539916992188</v>
       </c>
       <c r="BI3" s="2">
-        <v>5.6126728057861328</v>
+        <v>43.099933624267578</v>
       </c>
       <c r="BJ3" s="2">
-        <v>0</v>
+        <v>4.6816062927246094</v>
       </c>
       <c r="BK3" s="1">
         <v>1</v>
       </c>
       <c r="BL3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM3" s="2">
-        <v>18.734275817871094</v>
+        <v>18.21574592590332</v>
       </c>
       <c r="BN3" s="2">
-        <v>9.6759710311889648</v>
+        <v>42.9378662109375</v>
       </c>
       <c r="BO3" s="2">
-        <v>9.6759710311889648</v>
+        <v>7.8077750205993652</v>
       </c>
       <c r="BP3" s="2">
-        <v>0</v>
+        <v>35.130092620849609</v>
       </c>
       <c r="BQ3" s="2">
-        <v>14.227289199829102</v>
+        <v>14.384234428405762</v>
       </c>
       <c r="BR3" s="2">
-        <v>34.413803100585938</v>
+        <v>46.834102630615234</v>
       </c>
       <c r="BS3" s="2">
-        <v>20.556005477905273</v>
+        <v>3.9423618316650391</v>
       </c>
       <c r="BT3" s="2">
-        <v>13.857797622680664</v>
+        <v>42.891738891601563</v>
       </c>
       <c r="BU3" s="1">
-        <v>2.328934907913208</v>
+        <v>10.666536331176758</v>
       </c>
       <c r="BV3" s="1">
-        <v>8.7675819396972656</v>
+        <v>7.4639077186584473</v>
       </c>
       <c r="BW3" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
:pencil: ultima actualización de la sesión 8
</commit_message>
<xml_diff>
--- a/outputs/03-construccion-datos/duplicates/duplicates.xlsx
+++ b/outputs/03-construccion-datos/duplicates/duplicates.xlsx
@@ -581,10 +581,10 @@
         <v>1978</v>
       </c>
       <c r="K2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
@@ -593,148 +593,148 @@
         <v>0</v>
       </c>
       <c r="O2" s="2">
-        <v>13.250951766967773</v>
+        <v>5.7680816650390625</v>
       </c>
       <c r="P2" s="2">
-        <v>38.024566650390625</v>
+        <v>2.2352011203765869</v>
       </c>
       <c r="Q2" s="2">
-        <v>29.036596298217773</v>
+        <v>2.2352011203765869</v>
       </c>
       <c r="R2" s="2">
-        <v>8.9879703521728516</v>
+        <v>0</v>
       </c>
       <c r="S2" s="2">
-        <v>3.2160265445709229</v>
+        <v>19.658470153808594</v>
       </c>
       <c r="T2" s="2">
-        <v>35.548210144042969</v>
+        <v>42.728260040283203</v>
       </c>
       <c r="U2" s="2">
-        <v>8.6075477600097656</v>
+        <v>40.030673980712891</v>
       </c>
       <c r="V2" s="2">
-        <v>26.940662384033203</v>
+        <v>2.6975860595703125</v>
       </c>
       <c r="W2" s="1">
         <v>1</v>
       </c>
       <c r="X2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="2">
-        <v>17.446767807006836</v>
+        <v>16.939168930053711</v>
       </c>
       <c r="Z2" s="2">
-        <v>21.880966186523438</v>
+        <v>16.453506469726563</v>
       </c>
       <c r="AA2" s="2">
-        <v>1.1773288249969482</v>
+        <v>16.453506469726563</v>
       </c>
       <c r="AB2" s="2">
-        <v>20.703638076782227</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="2">
-        <v>8.8961515426635742</v>
+        <v>14.110039710998535</v>
       </c>
       <c r="AD2" s="2">
-        <v>2.1978754997253418</v>
+        <v>34.581287384033203</v>
       </c>
       <c r="AE2" s="2">
-        <v>2.1978754997253418</v>
+        <v>7.0867562294006348</v>
       </c>
       <c r="AF2" s="2">
-        <v>0</v>
+        <v>27.494531631469727</v>
       </c>
       <c r="AG2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH2" s="1">
         <v>0</v>
       </c>
       <c r="AI2" s="2">
-        <v>7.0325741767883301</v>
+        <v>4.0451245307922363</v>
       </c>
       <c r="AJ2" s="2">
-        <v>29.231773376464844</v>
+        <v>17.451549530029297</v>
       </c>
       <c r="AK2" s="2">
-        <v>29.231773376464844</v>
+        <v>17.451549530029297</v>
       </c>
       <c r="AL2" s="2">
         <v>0</v>
       </c>
       <c r="AM2" s="2">
-        <v>4.6432280540466309</v>
+        <v>2.4514777660369873</v>
       </c>
       <c r="AN2" s="2">
-        <v>8.4582910537719727</v>
+        <v>44.512004852294922</v>
       </c>
       <c r="AO2" s="2">
-        <v>8.4582910537719727</v>
+        <v>17.808340072631836</v>
       </c>
       <c r="AP2" s="2">
-        <v>0</v>
+        <v>26.703664779663086</v>
       </c>
       <c r="AQ2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR2" s="1">
         <v>0</v>
       </c>
       <c r="AS2" s="2">
-        <v>2.3537311553955078</v>
+        <v>3.6109740734100342</v>
       </c>
       <c r="AT2" s="2">
-        <v>32.880050659179688</v>
+        <v>27.876899719238281</v>
       </c>
       <c r="AU2" s="2">
-        <v>9.2514591217041016</v>
+        <v>20.809535980224609</v>
       </c>
       <c r="AV2" s="2">
-        <v>23.628591537475586</v>
+        <v>7.0673637390136719</v>
       </c>
       <c r="AW2" s="2">
-        <v>8.6124334335327148</v>
+        <v>9.8803443908691406</v>
       </c>
       <c r="AX2" s="2">
-        <v>13.234278678894043</v>
+        <v>8.5362758636474609</v>
       </c>
       <c r="AY2" s="2">
-        <v>13.234278678894043</v>
+        <v>8.5362758636474609</v>
       </c>
       <c r="AZ2" s="2">
         <v>0</v>
       </c>
       <c r="BA2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB2" s="1">
         <v>0</v>
       </c>
       <c r="BC2" s="2">
-        <v>1.9467545747756958</v>
+        <v>3.2463028430938721</v>
       </c>
       <c r="BD2" s="2">
-        <v>44.056102752685547</v>
+        <v>32.966930389404297</v>
       </c>
       <c r="BE2" s="2">
-        <v>39.308578491210938</v>
+        <v>32.966930389404297</v>
       </c>
       <c r="BF2" s="2">
-        <v>4.7475242614746094</v>
+        <v>0</v>
       </c>
       <c r="BG2" s="2">
-        <v>3.0712547302246094</v>
+        <v>8.0707817077636719</v>
       </c>
       <c r="BH2" s="2">
-        <v>47.781539916992188</v>
+        <v>11.795376777648926</v>
       </c>
       <c r="BI2" s="2">
-        <v>43.099933624267578</v>
+        <v>11.795376777648926</v>
       </c>
       <c r="BJ2" s="2">
-        <v>4.6816062927246094</v>
+        <v>0</v>
       </c>
       <c r="BK2" s="1">
         <v>1</v>
@@ -743,34 +743,34 @@
         <v>0</v>
       </c>
       <c r="BM2" s="2">
-        <v>18.21574592590332</v>
+        <v>5.4777421951293945</v>
       </c>
       <c r="BN2" s="2">
-        <v>42.9378662109375</v>
+        <v>44.768749237060547</v>
       </c>
       <c r="BO2" s="2">
-        <v>7.8077750205993652</v>
+        <v>5.536811351776123</v>
       </c>
       <c r="BP2" s="2">
-        <v>35.130092620849609</v>
+        <v>39.231937408447266</v>
       </c>
       <c r="BQ2" s="2">
-        <v>14.384234428405762</v>
+        <v>1.8907539844512939</v>
       </c>
       <c r="BR2" s="2">
-        <v>46.834102630615234</v>
+        <v>6.6376943588256836</v>
       </c>
       <c r="BS2" s="2">
-        <v>3.9423618316650391</v>
+        <v>3.558706521987915</v>
       </c>
       <c r="BT2" s="2">
-        <v>42.891738891601563</v>
+        <v>3.0789878368377686</v>
       </c>
       <c r="BU2" s="1">
-        <v>10.666536331176758</v>
+        <v>10.387241363525391</v>
       </c>
       <c r="BV2" s="1">
-        <v>7.4639077186584473</v>
+        <v>7.8235669136047363</v>
       </c>
       <c r="BW2" t="s">
         <v>86</v>
@@ -806,10 +806,10 @@
         <v>2036</v>
       </c>
       <c r="K3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M3" s="1">
         <v>0</v>
@@ -818,148 +818,148 @@
         <v>0</v>
       </c>
       <c r="O3" s="2">
-        <v>13.250951766967773</v>
+        <v>5.7680816650390625</v>
       </c>
       <c r="P3" s="2">
-        <v>38.024566650390625</v>
+        <v>2.2352011203765869</v>
       </c>
       <c r="Q3" s="2">
-        <v>29.036596298217773</v>
+        <v>2.2352011203765869</v>
       </c>
       <c r="R3" s="2">
-        <v>8.9879703521728516</v>
+        <v>0</v>
       </c>
       <c r="S3" s="2">
-        <v>3.2160265445709229</v>
+        <v>19.658470153808594</v>
       </c>
       <c r="T3" s="2">
-        <v>35.548210144042969</v>
+        <v>42.728260040283203</v>
       </c>
       <c r="U3" s="2">
-        <v>8.6075477600097656</v>
+        <v>40.030673980712891</v>
       </c>
       <c r="V3" s="2">
-        <v>26.940662384033203</v>
+        <v>2.6975860595703125</v>
       </c>
       <c r="W3" s="1">
         <v>1</v>
       </c>
       <c r="X3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3" s="2">
-        <v>17.446767807006836</v>
+        <v>16.939168930053711</v>
       </c>
       <c r="Z3" s="2">
-        <v>21.880966186523438</v>
+        <v>16.453506469726563</v>
       </c>
       <c r="AA3" s="2">
-        <v>1.1773288249969482</v>
+        <v>16.453506469726563</v>
       </c>
       <c r="AB3" s="2">
-        <v>20.703638076782227</v>
+        <v>0</v>
       </c>
       <c r="AC3" s="2">
-        <v>8.8961515426635742</v>
+        <v>14.110039710998535</v>
       </c>
       <c r="AD3" s="2">
-        <v>2.1978754997253418</v>
+        <v>34.581287384033203</v>
       </c>
       <c r="AE3" s="2">
-        <v>2.1978754997253418</v>
+        <v>7.0867562294006348</v>
       </c>
       <c r="AF3" s="2">
-        <v>0</v>
+        <v>27.494531631469727</v>
       </c>
       <c r="AG3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH3" s="1">
         <v>0</v>
       </c>
       <c r="AI3" s="2">
-        <v>7.0325741767883301</v>
+        <v>4.0451245307922363</v>
       </c>
       <c r="AJ3" s="2">
-        <v>29.231773376464844</v>
+        <v>17.451549530029297</v>
       </c>
       <c r="AK3" s="2">
-        <v>29.231773376464844</v>
+        <v>17.451549530029297</v>
       </c>
       <c r="AL3" s="2">
         <v>0</v>
       </c>
       <c r="AM3" s="2">
-        <v>4.6432280540466309</v>
+        <v>2.4514777660369873</v>
       </c>
       <c r="AN3" s="2">
-        <v>8.4582910537719727</v>
+        <v>44.512004852294922</v>
       </c>
       <c r="AO3" s="2">
-        <v>8.4582910537719727</v>
+        <v>17.808340072631836</v>
       </c>
       <c r="AP3" s="2">
-        <v>0</v>
+        <v>26.703664779663086</v>
       </c>
       <c r="AQ3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR3" s="1">
         <v>0</v>
       </c>
       <c r="AS3" s="2">
-        <v>2.3537311553955078</v>
+        <v>3.6109740734100342</v>
       </c>
       <c r="AT3" s="2">
-        <v>32.880050659179688</v>
+        <v>27.876899719238281</v>
       </c>
       <c r="AU3" s="2">
-        <v>9.2514591217041016</v>
+        <v>20.809535980224609</v>
       </c>
       <c r="AV3" s="2">
-        <v>23.628591537475586</v>
+        <v>7.0673637390136719</v>
       </c>
       <c r="AW3" s="2">
-        <v>8.6124334335327148</v>
+        <v>9.8803443908691406</v>
       </c>
       <c r="AX3" s="2">
-        <v>13.234278678894043</v>
+        <v>8.5362758636474609</v>
       </c>
       <c r="AY3" s="2">
-        <v>13.234278678894043</v>
+        <v>8.5362758636474609</v>
       </c>
       <c r="AZ3" s="2">
         <v>0</v>
       </c>
       <c r="BA3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB3" s="1">
         <v>0</v>
       </c>
       <c r="BC3" s="2">
-        <v>1.9467545747756958</v>
+        <v>3.2463028430938721</v>
       </c>
       <c r="BD3" s="2">
-        <v>44.056102752685547</v>
+        <v>32.966930389404297</v>
       </c>
       <c r="BE3" s="2">
-        <v>39.308578491210938</v>
+        <v>32.966930389404297</v>
       </c>
       <c r="BF3" s="2">
-        <v>4.7475242614746094</v>
+        <v>0</v>
       </c>
       <c r="BG3" s="2">
-        <v>3.0712547302246094</v>
+        <v>8.0707817077636719</v>
       </c>
       <c r="BH3" s="2">
-        <v>47.781539916992188</v>
+        <v>11.795376777648926</v>
       </c>
       <c r="BI3" s="2">
-        <v>43.099933624267578</v>
+        <v>11.795376777648926</v>
       </c>
       <c r="BJ3" s="2">
-        <v>4.6816062927246094</v>
+        <v>0</v>
       </c>
       <c r="BK3" s="1">
         <v>1</v>
@@ -968,34 +968,34 @@
         <v>0</v>
       </c>
       <c r="BM3" s="2">
-        <v>18.21574592590332</v>
+        <v>5.4777421951293945</v>
       </c>
       <c r="BN3" s="2">
-        <v>42.9378662109375</v>
+        <v>44.768749237060547</v>
       </c>
       <c r="BO3" s="2">
-        <v>7.8077750205993652</v>
+        <v>5.536811351776123</v>
       </c>
       <c r="BP3" s="2">
-        <v>35.130092620849609</v>
+        <v>39.231937408447266</v>
       </c>
       <c r="BQ3" s="2">
-        <v>14.384234428405762</v>
+        <v>1.8907539844512939</v>
       </c>
       <c r="BR3" s="2">
-        <v>46.834102630615234</v>
+        <v>6.6376943588256836</v>
       </c>
       <c r="BS3" s="2">
-        <v>3.9423618316650391</v>
+        <v>3.558706521987915</v>
       </c>
       <c r="BT3" s="2">
-        <v>42.891738891601563</v>
+        <v>3.0789878368377686</v>
       </c>
       <c r="BU3" s="1">
-        <v>10.666536331176758</v>
+        <v>10.387241363525391</v>
       </c>
       <c r="BV3" s="1">
-        <v>7.4639077186584473</v>
+        <v>7.8235669136047363</v>
       </c>
       <c r="BW3" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
:pencil: updated semana 3
</commit_message>
<xml_diff>
--- a/outputs/03-construccion-datos/duplicates/duplicates.xlsx
+++ b/outputs/03-construccion-datos/duplicates/duplicates.xlsx
@@ -24,7 +24,7 @@
     <t>datelisted</t>
   </si>
   <si>
-    <t>23Jan2021</t>
+    <t>29Jan2022</t>
   </si>
   <si>
     <t>datefixed</t>
@@ -581,10 +581,10 @@
         <v>1978</v>
       </c>
       <c r="K2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
@@ -593,148 +593,148 @@
         <v>0</v>
       </c>
       <c r="O2" s="2">
-        <v>5.7680816650390625</v>
+        <v>13.250951766967773</v>
       </c>
       <c r="P2" s="2">
-        <v>2.2352011203765869</v>
+        <v>38.024566650390625</v>
       </c>
       <c r="Q2" s="2">
-        <v>2.2352011203765869</v>
+        <v>29.036596298217773</v>
       </c>
       <c r="R2" s="2">
-        <v>0</v>
+        <v>8.9879703521728516</v>
       </c>
       <c r="S2" s="2">
-        <v>19.658470153808594</v>
+        <v>3.2160265445709229</v>
       </c>
       <c r="T2" s="2">
-        <v>42.728260040283203</v>
+        <v>35.548210144042969</v>
       </c>
       <c r="U2" s="2">
-        <v>40.030673980712891</v>
+        <v>8.6075477600097656</v>
       </c>
       <c r="V2" s="2">
-        <v>2.6975860595703125</v>
+        <v>26.940662384033203</v>
       </c>
       <c r="W2" s="1">
         <v>1</v>
       </c>
       <c r="X2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="2">
-        <v>16.939168930053711</v>
+        <v>17.446767807006836</v>
       </c>
       <c r="Z2" s="2">
-        <v>16.453506469726563</v>
+        <v>21.880966186523438</v>
       </c>
       <c r="AA2" s="2">
-        <v>16.453506469726563</v>
+        <v>1.1773288249969482</v>
       </c>
       <c r="AB2" s="2">
-        <v>0</v>
+        <v>20.703638076782227</v>
       </c>
       <c r="AC2" s="2">
-        <v>14.110039710998535</v>
+        <v>8.8961515426635742</v>
       </c>
       <c r="AD2" s="2">
-        <v>34.581287384033203</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AE2" s="2">
-        <v>7.0867562294006348</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AF2" s="2">
-        <v>27.494531631469727</v>
+        <v>0</v>
       </c>
       <c r="AG2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH2" s="1">
         <v>0</v>
       </c>
       <c r="AI2" s="2">
-        <v>4.0451245307922363</v>
+        <v>7.0325741767883301</v>
       </c>
       <c r="AJ2" s="2">
-        <v>17.451549530029297</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AK2" s="2">
-        <v>17.451549530029297</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AL2" s="2">
         <v>0</v>
       </c>
       <c r="AM2" s="2">
-        <v>2.4514777660369873</v>
+        <v>4.6432280540466309</v>
       </c>
       <c r="AN2" s="2">
-        <v>44.512004852294922</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AO2" s="2">
-        <v>17.808340072631836</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AP2" s="2">
-        <v>26.703664779663086</v>
+        <v>0</v>
       </c>
       <c r="AQ2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR2" s="1">
         <v>0</v>
       </c>
       <c r="AS2" s="2">
-        <v>3.6109740734100342</v>
+        <v>2.3537311553955078</v>
       </c>
       <c r="AT2" s="2">
-        <v>27.876899719238281</v>
+        <v>32.880050659179688</v>
       </c>
       <c r="AU2" s="2">
-        <v>20.809535980224609</v>
+        <v>9.2514591217041016</v>
       </c>
       <c r="AV2" s="2">
-        <v>7.0673637390136719</v>
+        <v>23.628591537475586</v>
       </c>
       <c r="AW2" s="2">
-        <v>9.8803443908691406</v>
+        <v>8.6124334335327148</v>
       </c>
       <c r="AX2" s="2">
-        <v>8.5362758636474609</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AY2" s="2">
-        <v>8.5362758636474609</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AZ2" s="2">
         <v>0</v>
       </c>
       <c r="BA2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB2" s="1">
         <v>0</v>
       </c>
       <c r="BC2" s="2">
-        <v>3.2463028430938721</v>
+        <v>1.9467545747756958</v>
       </c>
       <c r="BD2" s="2">
-        <v>32.966930389404297</v>
+        <v>44.056102752685547</v>
       </c>
       <c r="BE2" s="2">
-        <v>32.966930389404297</v>
+        <v>39.308578491210938</v>
       </c>
       <c r="BF2" s="2">
-        <v>0</v>
+        <v>4.7475242614746094</v>
       </c>
       <c r="BG2" s="2">
-        <v>8.0707817077636719</v>
+        <v>3.0712547302246094</v>
       </c>
       <c r="BH2" s="2">
-        <v>11.795376777648926</v>
+        <v>47.781539916992188</v>
       </c>
       <c r="BI2" s="2">
-        <v>11.795376777648926</v>
+        <v>43.099933624267578</v>
       </c>
       <c r="BJ2" s="2">
-        <v>0</v>
+        <v>4.6816062927246094</v>
       </c>
       <c r="BK2" s="1">
         <v>1</v>
@@ -743,34 +743,34 @@
         <v>0</v>
       </c>
       <c r="BM2" s="2">
-        <v>5.4777421951293945</v>
+        <v>18.21574592590332</v>
       </c>
       <c r="BN2" s="2">
-        <v>44.768749237060547</v>
+        <v>42.9378662109375</v>
       </c>
       <c r="BO2" s="2">
-        <v>5.536811351776123</v>
+        <v>7.8077750205993652</v>
       </c>
       <c r="BP2" s="2">
-        <v>39.231937408447266</v>
+        <v>35.130092620849609</v>
       </c>
       <c r="BQ2" s="2">
-        <v>1.8907539844512939</v>
+        <v>14.384234428405762</v>
       </c>
       <c r="BR2" s="2">
-        <v>6.6376943588256836</v>
+        <v>46.834102630615234</v>
       </c>
       <c r="BS2" s="2">
-        <v>3.558706521987915</v>
+        <v>3.9423618316650391</v>
       </c>
       <c r="BT2" s="2">
-        <v>3.0789878368377686</v>
+        <v>42.891738891601563</v>
       </c>
       <c r="BU2" s="1">
-        <v>10.387241363525391</v>
+        <v>10.666536331176758</v>
       </c>
       <c r="BV2" s="1">
-        <v>7.8235669136047363</v>
+        <v>7.4639077186584473</v>
       </c>
       <c r="BW2" t="s">
         <v>86</v>
@@ -806,10 +806,10 @@
         <v>2036</v>
       </c>
       <c r="K3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M3" s="1">
         <v>0</v>
@@ -818,148 +818,148 @@
         <v>0</v>
       </c>
       <c r="O3" s="2">
-        <v>5.7680816650390625</v>
+        <v>13.250951766967773</v>
       </c>
       <c r="P3" s="2">
-        <v>2.2352011203765869</v>
+        <v>38.024566650390625</v>
       </c>
       <c r="Q3" s="2">
-        <v>2.2352011203765869</v>
+        <v>29.036596298217773</v>
       </c>
       <c r="R3" s="2">
-        <v>0</v>
+        <v>8.9879703521728516</v>
       </c>
       <c r="S3" s="2">
-        <v>19.658470153808594</v>
+        <v>3.2160265445709229</v>
       </c>
       <c r="T3" s="2">
-        <v>42.728260040283203</v>
+        <v>35.548210144042969</v>
       </c>
       <c r="U3" s="2">
-        <v>40.030673980712891</v>
+        <v>8.6075477600097656</v>
       </c>
       <c r="V3" s="2">
-        <v>2.6975860595703125</v>
+        <v>26.940662384033203</v>
       </c>
       <c r="W3" s="1">
         <v>1</v>
       </c>
       <c r="X3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="2">
-        <v>16.939168930053711</v>
+        <v>17.446767807006836</v>
       </c>
       <c r="Z3" s="2">
-        <v>16.453506469726563</v>
+        <v>21.880966186523438</v>
       </c>
       <c r="AA3" s="2">
-        <v>16.453506469726563</v>
+        <v>1.1773288249969482</v>
       </c>
       <c r="AB3" s="2">
-        <v>0</v>
+        <v>20.703638076782227</v>
       </c>
       <c r="AC3" s="2">
-        <v>14.110039710998535</v>
+        <v>8.8961515426635742</v>
       </c>
       <c r="AD3" s="2">
-        <v>34.581287384033203</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AE3" s="2">
-        <v>7.0867562294006348</v>
+        <v>2.1978754997253418</v>
       </c>
       <c r="AF3" s="2">
-        <v>27.494531631469727</v>
+        <v>0</v>
       </c>
       <c r="AG3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH3" s="1">
         <v>0</v>
       </c>
       <c r="AI3" s="2">
-        <v>4.0451245307922363</v>
+        <v>7.0325741767883301</v>
       </c>
       <c r="AJ3" s="2">
-        <v>17.451549530029297</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AK3" s="2">
-        <v>17.451549530029297</v>
+        <v>29.231773376464844</v>
       </c>
       <c r="AL3" s="2">
         <v>0</v>
       </c>
       <c r="AM3" s="2">
-        <v>2.4514777660369873</v>
+        <v>4.6432280540466309</v>
       </c>
       <c r="AN3" s="2">
-        <v>44.512004852294922</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AO3" s="2">
-        <v>17.808340072631836</v>
+        <v>8.4582910537719727</v>
       </c>
       <c r="AP3" s="2">
-        <v>26.703664779663086</v>
+        <v>0</v>
       </c>
       <c r="AQ3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR3" s="1">
         <v>0</v>
       </c>
       <c r="AS3" s="2">
-        <v>3.6109740734100342</v>
+        <v>2.3537311553955078</v>
       </c>
       <c r="AT3" s="2">
-        <v>27.876899719238281</v>
+        <v>32.880050659179688</v>
       </c>
       <c r="AU3" s="2">
-        <v>20.809535980224609</v>
+        <v>9.2514591217041016</v>
       </c>
       <c r="AV3" s="2">
-        <v>7.0673637390136719</v>
+        <v>23.628591537475586</v>
       </c>
       <c r="AW3" s="2">
-        <v>9.8803443908691406</v>
+        <v>8.6124334335327148</v>
       </c>
       <c r="AX3" s="2">
-        <v>8.5362758636474609</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AY3" s="2">
-        <v>8.5362758636474609</v>
+        <v>13.234278678894043</v>
       </c>
       <c r="AZ3" s="2">
         <v>0</v>
       </c>
       <c r="BA3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB3" s="1">
         <v>0</v>
       </c>
       <c r="BC3" s="2">
-        <v>3.2463028430938721</v>
+        <v>1.9467545747756958</v>
       </c>
       <c r="BD3" s="2">
-        <v>32.966930389404297</v>
+        <v>44.056102752685547</v>
       </c>
       <c r="BE3" s="2">
-        <v>32.966930389404297</v>
+        <v>39.308578491210938</v>
       </c>
       <c r="BF3" s="2">
-        <v>0</v>
+        <v>4.7475242614746094</v>
       </c>
       <c r="BG3" s="2">
-        <v>8.0707817077636719</v>
+        <v>3.0712547302246094</v>
       </c>
       <c r="BH3" s="2">
-        <v>11.795376777648926</v>
+        <v>47.781539916992188</v>
       </c>
       <c r="BI3" s="2">
-        <v>11.795376777648926</v>
+        <v>43.099933624267578</v>
       </c>
       <c r="BJ3" s="2">
-        <v>0</v>
+        <v>4.6816062927246094</v>
       </c>
       <c r="BK3" s="1">
         <v>1</v>
@@ -968,34 +968,34 @@
         <v>0</v>
       </c>
       <c r="BM3" s="2">
-        <v>5.4777421951293945</v>
+        <v>18.21574592590332</v>
       </c>
       <c r="BN3" s="2">
-        <v>44.768749237060547</v>
+        <v>42.9378662109375</v>
       </c>
       <c r="BO3" s="2">
-        <v>5.536811351776123</v>
+        <v>7.8077750205993652</v>
       </c>
       <c r="BP3" s="2">
-        <v>39.231937408447266</v>
+        <v>35.130092620849609</v>
       </c>
       <c r="BQ3" s="2">
-        <v>1.8907539844512939</v>
+        <v>14.384234428405762</v>
       </c>
       <c r="BR3" s="2">
-        <v>6.6376943588256836</v>
+        <v>46.834102630615234</v>
       </c>
       <c r="BS3" s="2">
-        <v>3.558706521987915</v>
+        <v>3.9423618316650391</v>
       </c>
       <c r="BT3" s="2">
-        <v>3.0789878368377686</v>
+        <v>42.891738891601563</v>
       </c>
       <c r="BU3" s="1">
-        <v>10.387241363525391</v>
+        <v>10.666536331176758</v>
       </c>
       <c r="BV3" s="1">
-        <v>7.8235669136047363</v>
+        <v>7.4639077186584473</v>
       </c>
       <c r="BW3" t="s">
         <v>86</v>

</xml_diff>